<commit_message>
add full pub numbers and pub date
</commit_message>
<xml_diff>
--- a/citations.xlsx
+++ b/citations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="411">
   <si>
     <t>RAP - Citation ID</t>
   </si>
@@ -32,25 +32,40 @@
     <t>EPO - Citing patent Publication Number</t>
   </si>
   <si>
+    <t>EPO - Citing patent Publication Date</t>
+  </si>
+  <si>
     <t>EPO - Citing Application Number</t>
   </si>
   <si>
     <t>EPO - Citing Priority Number</t>
   </si>
   <si>
-    <t>EPO - Citing patent Application Type</t>
+    <t>EPO - Citing patent Application Type (type digit)</t>
   </si>
   <si>
     <t>EPO - Citing patent Application Country</t>
   </si>
   <si>
-    <t>104121059</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CN20141393790</t>
+    <t>EPO - Citing patent Application Kind</t>
+  </si>
+  <si>
+    <t>EPO - Citing patent Priority Date</t>
+  </si>
+  <si>
+    <t>CN104121059A  20140812</t>
+  </si>
+  <si>
+    <t>2014-10-29</t>
+  </si>
+  <si>
+    <t>201410393790</t>
+  </si>
+  <si>
+    <t>CN20141393790 20140812</t>
+  </si>
+  <si>
+    <t>patent for invention(1)</t>
   </si>
   <si>
     <t>CN</t>
@@ -62,376 +77,607 @@
     <t>2014-08-12</t>
   </si>
   <si>
-    <t>104401401</t>
-  </si>
-  <si>
-    <t>CN20141697552</t>
+    <t>CN104401401A  20141126</t>
+  </si>
+  <si>
+    <t>2015-03-11</t>
+  </si>
+  <si>
+    <t>201410697552</t>
+  </si>
+  <si>
+    <t>CN20141697552 20141126</t>
   </si>
   <si>
     <t>2014-11-26</t>
   </si>
   <si>
-    <t>104051921</t>
-  </si>
-  <si>
-    <t>CN20141301371</t>
+    <t>CN104051921A  20140627</t>
+  </si>
+  <si>
+    <t>2014-09-17</t>
+  </si>
+  <si>
+    <t>201410301371</t>
+  </si>
+  <si>
+    <t>CN20141301371 20140627</t>
   </si>
   <si>
     <t>2014-06-27</t>
   </si>
   <si>
-    <t>103801871</t>
-  </si>
-  <si>
-    <t>CN20121445426</t>
+    <t>CN103801871A  20121109</t>
+  </si>
+  <si>
+    <t>2014-05-21</t>
+  </si>
+  <si>
+    <t>201210445426</t>
+  </si>
+  <si>
+    <t>CN20121445426 20121109</t>
   </si>
   <si>
     <t>2012-11-09</t>
   </si>
   <si>
-    <t>103802913</t>
-  </si>
-  <si>
-    <t>CN20121442369</t>
+    <t>CN103802913A  20121108</t>
+  </si>
+  <si>
+    <t>201210442369</t>
+  </si>
+  <si>
+    <t>CN20121442369 20121108</t>
   </si>
   <si>
     <t>2012-11-08</t>
   </si>
   <si>
-    <t>103358877</t>
-  </si>
-  <si>
-    <t>CN20121102922</t>
+    <t>CN103358877A  20120410</t>
+  </si>
+  <si>
+    <t>2013-10-23</t>
+  </si>
+  <si>
+    <t>201210102922</t>
+  </si>
+  <si>
+    <t>CN20121102922 20120410</t>
   </si>
   <si>
     <t>2012-04-10</t>
   </si>
   <si>
-    <t>103072558</t>
-  </si>
-  <si>
-    <t>CN2013150506</t>
+    <t>CN103072558A  20130215</t>
+  </si>
+  <si>
+    <t>2013-05-01</t>
+  </si>
+  <si>
+    <t>201310050506</t>
+  </si>
+  <si>
+    <t>CN2013150506 20130215</t>
   </si>
   <si>
     <t>2013-02-15</t>
   </si>
   <si>
-    <t>103693024</t>
-  </si>
-  <si>
-    <t>CN20131629488</t>
+    <t>CN103693024A  20131128</t>
+  </si>
+  <si>
+    <t>2014-04-02</t>
+  </si>
+  <si>
+    <t>201310629488</t>
+  </si>
+  <si>
+    <t>CN20131629488 20131128</t>
   </si>
   <si>
     <t>2013-11-28</t>
   </si>
   <si>
-    <t>104417382</t>
-  </si>
-  <si>
-    <t>CN20131389502</t>
+    <t>CN104417382A  20130830</t>
+  </si>
+  <si>
+    <t>2015-03-18</t>
+  </si>
+  <si>
+    <t>201310389502</t>
+  </si>
+  <si>
+    <t>CN20131389502 20130830</t>
   </si>
   <si>
     <t>2013-08-30</t>
   </si>
   <si>
-    <t>104417504</t>
-  </si>
-  <si>
-    <t>CN20131389431</t>
-  </si>
-  <si>
-    <t>102799166</t>
-  </si>
-  <si>
-    <t>CN20121295338</t>
+    <t>CN104417504A  20130830</t>
+  </si>
+  <si>
+    <t>201310389431</t>
+  </si>
+  <si>
+    <t>CN20131389431 20130830</t>
+  </si>
+  <si>
+    <t>CN102799166A  20120817</t>
+  </si>
+  <si>
+    <t>2012-11-28</t>
+  </si>
+  <si>
+    <t>201210295338</t>
+  </si>
+  <si>
+    <t>CN20121295338 20120817</t>
   </si>
   <si>
     <t>2012-08-17</t>
   </si>
   <si>
-    <t>102897170</t>
-  </si>
-  <si>
-    <t>CN20121447889</t>
-  </si>
-  <si>
-    <t>103192734</t>
-  </si>
-  <si>
-    <t>CN2013190182</t>
+    <t>CN102897170A  20121109</t>
+  </si>
+  <si>
+    <t>2013-01-30</t>
+  </si>
+  <si>
+    <t>201210447889</t>
+  </si>
+  <si>
+    <t>CN20121447889 20121109</t>
+  </si>
+  <si>
+    <t>CN103192734A  20130320</t>
+  </si>
+  <si>
+    <t>2013-07-10</t>
+  </si>
+  <si>
+    <t>201310090182</t>
+  </si>
+  <si>
+    <t>CN2013190182 20130320</t>
   </si>
   <si>
     <t>2013-03-20</t>
   </si>
   <si>
-    <t>103660970</t>
-  </si>
-  <si>
-    <t>CN2014107655</t>
+    <t>CN103660970A  20140108</t>
+  </si>
+  <si>
+    <t>2014-03-26</t>
+  </si>
+  <si>
+    <t>201410007655</t>
+  </si>
+  <si>
+    <t>CN2014107655 20140108</t>
   </si>
   <si>
     <t>2014-01-08</t>
   </si>
   <si>
-    <t>103863300</t>
-  </si>
-  <si>
-    <t>CN20121526426</t>
+    <t>CN103863300A  20121207</t>
+  </si>
+  <si>
+    <t>2014-06-18</t>
+  </si>
+  <si>
+    <t>201210526426</t>
+  </si>
+  <si>
+    <t>CN20121526426 20121207</t>
   </si>
   <si>
     <t>2012-12-07</t>
   </si>
   <si>
-    <t>103935226</t>
-  </si>
-  <si>
-    <t>CN20141161237</t>
+    <t>CN103935226A  20140422</t>
+  </si>
+  <si>
+    <t>2014-07-23</t>
+  </si>
+  <si>
+    <t>201410161237</t>
+  </si>
+  <si>
+    <t>CN20141161237 20140422</t>
   </si>
   <si>
     <t>2014-04-22</t>
   </si>
   <si>
-    <t>104393661</t>
-  </si>
-  <si>
-    <t>CN20141757979</t>
+    <t>CN104393661A  20141212</t>
+  </si>
+  <si>
+    <t>2015-03-04</t>
+  </si>
+  <si>
+    <t>201410757979</t>
+  </si>
+  <si>
+    <t>CN20141757979 20141212</t>
   </si>
   <si>
     <t>2014-12-12</t>
   </si>
   <si>
-    <t>104590041</t>
-  </si>
-  <si>
-    <t>CN20141698950</t>
+    <t>CN104590041A  20141128</t>
+  </si>
+  <si>
+    <t>2015-05-06</t>
+  </si>
+  <si>
+    <t>201410698950</t>
+  </si>
+  <si>
+    <t>CN20141698950 20141128</t>
   </si>
   <si>
     <t>2014-11-28</t>
   </si>
   <si>
-    <t>102497139</t>
-  </si>
-  <si>
-    <t>CN20111394025</t>
+    <t>CN102497139A  20111202</t>
+  </si>
+  <si>
+    <t>2012-06-13</t>
+  </si>
+  <si>
+    <t>201110394025</t>
+  </si>
+  <si>
+    <t>CN20111394025 20111202</t>
   </si>
   <si>
     <t>2011-12-02</t>
   </si>
   <si>
-    <t>103747550</t>
-  </si>
-  <si>
-    <t>CN2014123897</t>
+    <t>CN103747550A  20140117</t>
+  </si>
+  <si>
+    <t>2014-04-23</t>
+  </si>
+  <si>
+    <t>201410023897</t>
+  </si>
+  <si>
+    <t>CN2014123897 20140117</t>
   </si>
   <si>
     <t>2014-01-17</t>
   </si>
   <si>
-    <t>102425877</t>
-  </si>
-  <si>
-    <t>CN20111427819</t>
+    <t>CN102425877A  20111219</t>
+  </si>
+  <si>
+    <t>2012-04-25</t>
+  </si>
+  <si>
+    <t>201110427819</t>
+  </si>
+  <si>
+    <t>CN20111427819 20111219</t>
   </si>
   <si>
     <t>2011-12-19</t>
   </si>
   <si>
-    <t>103115400</t>
-  </si>
-  <si>
-    <t>CN2013178034</t>
+    <t>CN103115400A  20130312</t>
+  </si>
+  <si>
+    <t>2013-05-22</t>
+  </si>
+  <si>
+    <t>201310078034</t>
+  </si>
+  <si>
+    <t>CN2013178034 20130312</t>
   </si>
   <si>
     <t>2013-03-12</t>
   </si>
   <si>
-    <t>103644617</t>
-  </si>
-  <si>
-    <t>CN20131751248</t>
+    <t>CN103644617A  20131230</t>
+  </si>
+  <si>
+    <t>2014-03-19</t>
+  </si>
+  <si>
+    <t>201310751248</t>
+  </si>
+  <si>
+    <t>CN20131751248 20131230</t>
   </si>
   <si>
     <t>2013-12-30</t>
   </si>
   <si>
-    <t>103692880</t>
-  </si>
-  <si>
-    <t>CN20121368510</t>
+    <t>CN103692880A  20120928</t>
+  </si>
+  <si>
+    <t>201210368510</t>
+  </si>
+  <si>
+    <t>CN20121368510 20120928</t>
   </si>
   <si>
     <t>2012-09-28</t>
   </si>
   <si>
-    <t>102392885</t>
-  </si>
-  <si>
-    <t>CN20111173011</t>
+    <t>CN102392885A  20110624</t>
+  </si>
+  <si>
+    <t>2012-03-28</t>
+  </si>
+  <si>
+    <t>201110173011</t>
+  </si>
+  <si>
+    <t>CN20111173011 20110624</t>
   </si>
   <si>
     <t>2011-06-24</t>
   </si>
   <si>
-    <t>102518780</t>
-  </si>
-  <si>
-    <t>CN20111423147</t>
+    <t>CN102518780A  20111216</t>
+  </si>
+  <si>
+    <t>2012-06-27</t>
+  </si>
+  <si>
+    <t>201110423147</t>
+  </si>
+  <si>
+    <t>CN20111423147 20111216</t>
   </si>
   <si>
     <t>2011-12-16</t>
   </si>
   <si>
-    <t>102700407</t>
-  </si>
-  <si>
-    <t>CN20121185035</t>
+    <t>CN102700407A  20120606</t>
+  </si>
+  <si>
+    <t>2012-10-03</t>
+  </si>
+  <si>
+    <t>201210185035</t>
+  </si>
+  <si>
+    <t>CN20121185035 20120606</t>
   </si>
   <si>
     <t>2012-06-06</t>
   </si>
   <si>
-    <t>102700409</t>
-  </si>
-  <si>
-    <t>CN20121185054</t>
-  </si>
-  <si>
-    <t>102678893</t>
-  </si>
-  <si>
-    <t>CN20121171412</t>
+    <t>CN102700409A  20120606</t>
+  </si>
+  <si>
+    <t>201210185054</t>
+  </si>
+  <si>
+    <t>CN20121185054 20120606</t>
+  </si>
+  <si>
+    <t>CN102678893A  20120529</t>
+  </si>
+  <si>
+    <t>2012-09-19</t>
+  </si>
+  <si>
+    <t>201210171412</t>
+  </si>
+  <si>
+    <t>CN20121171412 20120529</t>
   </si>
   <si>
     <t>2012-05-29</t>
   </si>
   <si>
-    <t>102678850</t>
-  </si>
-  <si>
-    <t>CN20121136145</t>
+    <t>CN102678850A  20120504</t>
+  </si>
+  <si>
+    <t>201210136145</t>
+  </si>
+  <si>
+    <t>CN20121136145 20120504</t>
   </si>
   <si>
     <t>2012-05-04</t>
   </si>
   <si>
-    <t>102826191</t>
-  </si>
-  <si>
-    <t>CN20121364259</t>
+    <t>CN102826191A  20120926</t>
+  </si>
+  <si>
+    <t>2012-12-19</t>
+  </si>
+  <si>
+    <t>201210364259</t>
+  </si>
+  <si>
+    <t>CN20121364259 20120926</t>
   </si>
   <si>
     <t>2012-09-26</t>
   </si>
   <si>
-    <t>103307222</t>
-  </si>
-  <si>
-    <t>CN20131234496</t>
+    <t>CN103307222A  20130613</t>
+  </si>
+  <si>
+    <t>2013-09-18</t>
+  </si>
+  <si>
+    <t>201310234496</t>
+  </si>
+  <si>
+    <t>CN20131234496 20130613</t>
   </si>
   <si>
     <t>2013-06-13</t>
   </si>
   <si>
-    <t>103307223</t>
-  </si>
-  <si>
-    <t>CN2012158850</t>
+    <t>CN103307223A  20120308</t>
+  </si>
+  <si>
+    <t>201210058850</t>
+  </si>
+  <si>
+    <t>CN2012158850 20120308</t>
   </si>
   <si>
     <t>2012-03-08</t>
   </si>
   <si>
-    <t>103438173</t>
-  </si>
-  <si>
-    <t>CN20131402944</t>
+    <t>CN103438173A  20130906</t>
+  </si>
+  <si>
+    <t>2013-12-11</t>
+  </si>
+  <si>
+    <t>201310402944</t>
+  </si>
+  <si>
+    <t>CN20131402944 20130906</t>
   </si>
   <si>
     <t>2013-09-06</t>
   </si>
   <si>
-    <t>103851183</t>
-  </si>
-  <si>
-    <t>CN20121522171</t>
-  </si>
-  <si>
-    <t>102733960</t>
-  </si>
-  <si>
-    <t>CN2011182486</t>
+    <t>CN103851183A  20121207</t>
+  </si>
+  <si>
+    <t>2014-06-11</t>
+  </si>
+  <si>
+    <t>201210522171</t>
+  </si>
+  <si>
+    <t>CN20121522171 20121207</t>
+  </si>
+  <si>
+    <t>CN102733960A  20110401</t>
+  </si>
+  <si>
+    <t>2012-10-17</t>
+  </si>
+  <si>
+    <t>201110082486</t>
+  </si>
+  <si>
+    <t>CN2011182486 20110401</t>
   </si>
   <si>
     <t>2011-04-01</t>
   </si>
   <si>
-    <t>102808714</t>
-  </si>
-  <si>
-    <t>CN20121265473</t>
+    <t>CN102808714A  20120728</t>
+  </si>
+  <si>
+    <t>2012-12-05</t>
+  </si>
+  <si>
+    <t>201210265473</t>
+  </si>
+  <si>
+    <t>CN20121265473 20120728</t>
   </si>
   <si>
     <t>2012-07-28</t>
   </si>
   <si>
-    <t>103850811</t>
-  </si>
-  <si>
-    <t>CN20131610800</t>
+    <t>CN103850811A  20131126</t>
+  </si>
+  <si>
+    <t>201310610800</t>
+  </si>
+  <si>
+    <t>CN20131610800 20131126</t>
   </si>
   <si>
     <t>2013-11-26</t>
   </si>
   <si>
-    <t>102523724</t>
-  </si>
-  <si>
-    <t>CN20111400184</t>
+    <t>CN102523724A  20111206</t>
+  </si>
+  <si>
+    <t>201110400184</t>
+  </si>
+  <si>
+    <t>CN20111400184 20111206</t>
   </si>
   <si>
     <t>2011-12-06</t>
   </si>
   <si>
-    <t>102951012</t>
-  </si>
-  <si>
-    <t>CN20111253231</t>
+    <t>CN102951012A  20110830</t>
+  </si>
+  <si>
+    <t>2013-03-06</t>
+  </si>
+  <si>
+    <t>201110253231</t>
+  </si>
+  <si>
+    <t>CN20111253231 20110830</t>
   </si>
   <si>
     <t>2011-08-30</t>
   </si>
   <si>
-    <t>102529641</t>
-  </si>
-  <si>
-    <t>CN20111361431</t>
+    <t>CN102529641A  20111115</t>
+  </si>
+  <si>
+    <t>2012-07-04</t>
+  </si>
+  <si>
+    <t>201110361431</t>
+  </si>
+  <si>
+    <t>CN20111361431 20111115</t>
   </si>
   <si>
     <t>2011-11-15</t>
   </si>
   <si>
-    <t>104044434</t>
-  </si>
-  <si>
-    <t>CN20141325714</t>
+    <t>CN104044434A  20140710</t>
+  </si>
+  <si>
+    <t>201410325714</t>
+  </si>
+  <si>
+    <t>CN20141325714 20140710</t>
   </si>
   <si>
     <t>2014-07-10</t>
   </si>
   <si>
-    <t>102381302</t>
-  </si>
-  <si>
-    <t>CN20111241614</t>
+    <t>CN102381302A  20110823</t>
+  </si>
+  <si>
+    <t>2012-03-21</t>
+  </si>
+  <si>
+    <t>201110241614</t>
+  </si>
+  <si>
+    <t>CN20111241614 20110823</t>
   </si>
   <si>
     <t>2011-08-23</t>
   </si>
   <si>
-    <t>2492404</t>
-  </si>
-  <si>
-    <t>GB20110011231</t>
+    <t>GB2492404A  20110701</t>
+  </si>
+  <si>
+    <t>2013-01-02</t>
+  </si>
+  <si>
+    <t>201111231</t>
+  </si>
+  <si>
+    <t>GB20110011231 20110701</t>
   </si>
   <si>
     <t>GB</t>
@@ -440,181 +686,295 @@
     <t>2011-07-01</t>
   </si>
   <si>
-    <t>102806900</t>
-  </si>
-  <si>
-    <t>CN20121290307</t>
+    <t>CN102806900A  20120816</t>
+  </si>
+  <si>
+    <t>201210290307</t>
+  </si>
+  <si>
+    <t>CN20121290307 20120816</t>
   </si>
   <si>
     <t>2012-08-16</t>
   </si>
   <si>
-    <t>103158690</t>
-  </si>
-  <si>
-    <t>CN20111425518</t>
-  </si>
-  <si>
-    <t>103693033</t>
-  </si>
-  <si>
-    <t>CN20121369313</t>
+    <t>CN103158690A  20111216</t>
+  </si>
+  <si>
+    <t>2013-06-19</t>
+  </si>
+  <si>
+    <t>201110425518</t>
+  </si>
+  <si>
+    <t>CN20111425518 20111216</t>
+  </si>
+  <si>
+    <t>2014-03-12</t>
+  </si>
+  <si>
+    <t>CN103693033A  20120927</t>
+  </si>
+  <si>
+    <t>201210369313</t>
+  </si>
+  <si>
+    <t>CN20121369313 20120927</t>
   </si>
   <si>
     <t>2012-09-27</t>
   </si>
   <si>
-    <t>103723137</t>
-  </si>
-  <si>
-    <t>CN20131739330</t>
-  </si>
-  <si>
-    <t>102320334</t>
-  </si>
-  <si>
-    <t>CN20111162862</t>
+    <t>CN103723137A  20131230</t>
+  </si>
+  <si>
+    <t>2014-04-16</t>
+  </si>
+  <si>
+    <t>201310739330</t>
+  </si>
+  <si>
+    <t>CN20131739330 20131230</t>
+  </si>
+  <si>
+    <t>CN102320334A  20110617</t>
+  </si>
+  <si>
+    <t>2012-01-18</t>
+  </si>
+  <si>
+    <t>201110162862</t>
+  </si>
+  <si>
+    <t>CN20111162862 20110617</t>
   </si>
   <si>
     <t>2011-06-17</t>
   </si>
   <si>
-    <t>102530105</t>
-  </si>
-  <si>
-    <t>CN20111449465</t>
+    <t>CN102530105A  20111228</t>
+  </si>
+  <si>
+    <t>201110449465</t>
+  </si>
+  <si>
+    <t>CN20111449465 20111228</t>
   </si>
   <si>
     <t>2011-12-28</t>
   </si>
   <si>
-    <t>103556663</t>
-  </si>
-  <si>
-    <t>CN20131542289</t>
+    <t>CN103556663A  20131105</t>
+  </si>
+  <si>
+    <t>2014-02-05</t>
+  </si>
+  <si>
+    <t>201310542289</t>
+  </si>
+  <si>
+    <t>CN20131542289 20131105</t>
   </si>
   <si>
     <t>2013-11-05</t>
   </si>
   <si>
-    <t>102116242</t>
-  </si>
-  <si>
-    <t>CN20101615738</t>
+    <t>CN102116242A  20101230</t>
+  </si>
+  <si>
+    <t>2011-07-06</t>
+  </si>
+  <si>
+    <t>201010615738</t>
+  </si>
+  <si>
+    <t>CN20101615738 20101230</t>
   </si>
   <si>
     <t>2010-12-30</t>
   </si>
   <si>
-    <t>103388528</t>
-  </si>
-  <si>
-    <t>CN20131147871</t>
+    <t>CN103388528A  20130425</t>
+  </si>
+  <si>
+    <t>2013-11-13</t>
+  </si>
+  <si>
+    <t>201310147871</t>
+  </si>
+  <si>
+    <t>CN20131147871 20130425</t>
   </si>
   <si>
     <t>2013-04-25</t>
   </si>
   <si>
-    <t>102606267</t>
-  </si>
-  <si>
-    <t>CN2012118596</t>
+    <t>CN102606267A  20120120</t>
+  </si>
+  <si>
+    <t>2012-07-25</t>
+  </si>
+  <si>
+    <t>201210018596</t>
+  </si>
+  <si>
+    <t>CN2012118596 20120120</t>
   </si>
   <si>
     <t>2012-01-20</t>
   </si>
   <si>
-    <t>102966419</t>
-  </si>
-  <si>
-    <t>CN20121314570</t>
+    <t>CN102966419A  20120830</t>
+  </si>
+  <si>
+    <t>2013-03-13</t>
+  </si>
+  <si>
+    <t>201210314570</t>
+  </si>
+  <si>
+    <t>CN20121314570 20120830</t>
   </si>
   <si>
     <t>2012-08-30</t>
   </si>
   <si>
-    <t>104279036</t>
-  </si>
-  <si>
-    <t>CN20141439812</t>
+    <t>CN104279036A  20140901</t>
+  </si>
+  <si>
+    <t>2015-01-14</t>
+  </si>
+  <si>
+    <t>201410439812</t>
+  </si>
+  <si>
+    <t>CN20141439812 20140901</t>
   </si>
   <si>
     <t>2014-09-01</t>
   </si>
   <si>
-    <t>102145652</t>
-  </si>
-  <si>
-    <t>CN2011129586</t>
+    <t>CN102145652A  20110126</t>
+  </si>
+  <si>
+    <t>2011-08-10</t>
+  </si>
+  <si>
+    <t>201110029586</t>
+  </si>
+  <si>
+    <t>CN2011129586 20110126</t>
   </si>
   <si>
     <t>2011-01-26</t>
   </si>
   <si>
-    <t>104648172</t>
-  </si>
-  <si>
-    <t>CN2015164911</t>
+    <t>CN104648172A  20150203</t>
+  </si>
+  <si>
+    <t>2015-05-27</t>
+  </si>
+  <si>
+    <t>201510064911</t>
+  </si>
+  <si>
+    <t>CN2015164911 20150203</t>
   </si>
   <si>
     <t>2015-02-03</t>
   </si>
   <si>
-    <t>103465899</t>
-  </si>
-  <si>
-    <t>CN20131435150</t>
+    <t>CN103465899A  20130923</t>
+  </si>
+  <si>
+    <t>2013-12-25</t>
+  </si>
+  <si>
+    <t>201310435150</t>
+  </si>
+  <si>
+    <t>CN20131435150 20130923</t>
   </si>
   <si>
     <t>2013-09-23</t>
   </si>
   <si>
-    <t>103775265</t>
-  </si>
-  <si>
-    <t>CN2014140221</t>
+    <t>CN103775265A  20140127</t>
+  </si>
+  <si>
+    <t>2014-05-07</t>
+  </si>
+  <si>
+    <t>201410040221</t>
+  </si>
+  <si>
+    <t>CN2014140221 20140127</t>
   </si>
   <si>
     <t>2014-01-27</t>
   </si>
   <si>
-    <t>103867307</t>
-  </si>
-  <si>
-    <t>CN20141128265</t>
-  </si>
-  <si>
-    <t>2014-04-02</t>
-  </si>
-  <si>
-    <t>103035058</t>
-  </si>
-  <si>
-    <t>CN20121525964</t>
-  </si>
-  <si>
-    <t>103684753</t>
-  </si>
-  <si>
-    <t>CN20131640810</t>
+    <t>CN103867307A  20140402</t>
+  </si>
+  <si>
+    <t>201410128265</t>
+  </si>
+  <si>
+    <t>CN20141128265 20140402</t>
+  </si>
+  <si>
+    <t>CN103035058A  20121207</t>
+  </si>
+  <si>
+    <t>2013-04-10</t>
+  </si>
+  <si>
+    <t>201210525964</t>
+  </si>
+  <si>
+    <t>CN20121525964 20121207</t>
+  </si>
+  <si>
+    <t>CN103684753A  20131204</t>
+  </si>
+  <si>
+    <t>201310640810</t>
+  </si>
+  <si>
+    <t>CN20131640810 20131204</t>
   </si>
   <si>
     <t>2013-12-04</t>
   </si>
   <si>
-    <t>103714483</t>
-  </si>
-  <si>
-    <t>CN20131690753</t>
+    <t>CN103714483A  20131215</t>
+  </si>
+  <si>
+    <t>2014-04-09</t>
+  </si>
+  <si>
+    <t>201310690753</t>
+  </si>
+  <si>
+    <t>CN20131690753 20131215</t>
   </si>
   <si>
     <t>2013-12-15</t>
   </si>
   <si>
-    <t>2009094949</t>
-  </si>
-  <si>
-    <t>WO2009CN70305</t>
+    <t>CN2009094949W  20090123</t>
+  </si>
+  <si>
+    <t>2009-08-06</t>
+  </si>
+  <si>
+    <t>2009070305</t>
+  </si>
+  <si>
+    <t>WO2009CN70305 20090123</t>
+  </si>
+  <si>
+    <t>Undefined type(0)</t>
   </si>
   <si>
     <t xml:space="preserve">W </t>
@@ -623,172 +983,265 @@
     <t>2009-01-23</t>
   </si>
   <si>
-    <t>101986337</t>
-  </si>
-  <si>
-    <t>CN20101526498</t>
+    <t>CN101986337A  20101029</t>
+  </si>
+  <si>
+    <t>2011-03-16</t>
+  </si>
+  <si>
+    <t>201010526498</t>
+  </si>
+  <si>
+    <t>CN20101526498 20101029</t>
   </si>
   <si>
     <t>2010-10-29</t>
   </si>
   <si>
-    <t>102957714</t>
-  </si>
-  <si>
-    <t>CN20111237392</t>
+    <t>CN102957714A  20110818</t>
+  </si>
+  <si>
+    <t>201110237392</t>
+  </si>
+  <si>
+    <t>CN20111237392 20110818</t>
   </si>
   <si>
     <t>2011-08-18</t>
   </si>
   <si>
-    <t>102368321</t>
-  </si>
-  <si>
-    <t>CN20111338522</t>
+    <t>CN102368321A  20111101</t>
+  </si>
+  <si>
+    <t>2012-03-07</t>
+  </si>
+  <si>
+    <t>201110338522</t>
+  </si>
+  <si>
+    <t>CN20111338522 20111101</t>
   </si>
   <si>
     <t>2011-11-01</t>
   </si>
   <si>
-    <t>102800018</t>
-  </si>
-  <si>
-    <t>CN20121236949</t>
+    <t>CN102800018A  20120709</t>
+  </si>
+  <si>
+    <t>201210236949</t>
+  </si>
+  <si>
+    <t>CN20121236949 20120709</t>
   </si>
   <si>
     <t>2012-07-09</t>
   </si>
   <si>
-    <t>103164753</t>
-  </si>
-  <si>
-    <t>CN20111405109</t>
+    <t>CN103164753A  20111208</t>
+  </si>
+  <si>
+    <t>201110405109</t>
+  </si>
+  <si>
+    <t>CN20111405109 20111208</t>
   </si>
   <si>
     <t>2011-12-08</t>
   </si>
   <si>
-    <t>2014161136</t>
-  </si>
-  <si>
-    <t>WO2013CN73566</t>
+    <t>CN2014161136W  20130401</t>
+  </si>
+  <si>
+    <t>2014-10-09</t>
+  </si>
+  <si>
+    <t>2013073566</t>
+  </si>
+  <si>
+    <t>WO2013CN73566 20130401</t>
   </si>
   <si>
     <t>2013-04-01</t>
   </si>
   <si>
-    <t>102663650</t>
-  </si>
-  <si>
-    <t>CN2012166710</t>
+    <t>CN102663650A  20120314</t>
+  </si>
+  <si>
+    <t>2012-09-12</t>
+  </si>
+  <si>
+    <t>201210066710</t>
+  </si>
+  <si>
+    <t>CN2012166710 20120314</t>
   </si>
   <si>
     <t>2012-03-14</t>
   </si>
   <si>
-    <t>102779297</t>
-  </si>
-  <si>
-    <t>CN20121217622</t>
+    <t>CN102779297A  20120628</t>
+  </si>
+  <si>
+    <t>2012-11-14</t>
+  </si>
+  <si>
+    <t>201210217622</t>
+  </si>
+  <si>
+    <t>CN20121217622 20120628</t>
   </si>
   <si>
     <t>2012-06-28</t>
   </si>
   <si>
-    <t>103123712</t>
-  </si>
-  <si>
-    <t>CN20111366881</t>
+    <t>CN103123712A  20111117</t>
+  </si>
+  <si>
+    <t>2013-05-29</t>
+  </si>
+  <si>
+    <t>201110366881</t>
+  </si>
+  <si>
+    <t>CN20111366881 20111117</t>
   </si>
   <si>
     <t>2011-11-17</t>
   </si>
   <si>
-    <t>102332140</t>
-  </si>
-  <si>
-    <t>CN20101229253</t>
+    <t>CN102332140A  20100712</t>
+  </si>
+  <si>
+    <t>2012-01-25</t>
+  </si>
+  <si>
+    <t>201010229253</t>
+  </si>
+  <si>
+    <t>CN20101229253 20100712</t>
   </si>
   <si>
     <t>2010-07-12</t>
   </si>
   <si>
-    <t>102487378</t>
-  </si>
-  <si>
-    <t>CN20101568405</t>
+    <t>CN102487378A  20101201</t>
+  </si>
+  <si>
+    <t>201010568405</t>
+  </si>
+  <si>
+    <t>CN20101568405 20101201</t>
   </si>
   <si>
     <t>2010-12-01</t>
   </si>
   <si>
-    <t>102542423</t>
-  </si>
-  <si>
-    <t>CN20101579532</t>
+    <t>CN102542423A  20101208</t>
+  </si>
+  <si>
+    <t>201010579532</t>
+  </si>
+  <si>
+    <t>CN20101579532 20101208</t>
   </si>
   <si>
     <t>2010-12-08</t>
   </si>
   <si>
-    <t>2013107181</t>
-  </si>
-  <si>
-    <t>WO2012CN80775</t>
-  </si>
-  <si>
-    <t>102045365</t>
-  </si>
-  <si>
-    <t>CN20101624551</t>
-  </si>
-  <si>
-    <t>102521778</t>
-  </si>
-  <si>
-    <t>CN20111407040</t>
-  </si>
-  <si>
-    <t>103078911</t>
-  </si>
-  <si>
-    <t>CN20121580153</t>
+    <t>CN2013107181W  20120830</t>
+  </si>
+  <si>
+    <t>2013-07-25</t>
+  </si>
+  <si>
+    <t>2012080775</t>
+  </si>
+  <si>
+    <t>WO2012CN80775 20120830</t>
+  </si>
+  <si>
+    <t>CN102045365A  20101230</t>
+  </si>
+  <si>
+    <t>2011-05-04</t>
+  </si>
+  <si>
+    <t>201010624551</t>
+  </si>
+  <si>
+    <t>CN20101624551 20101230</t>
+  </si>
+  <si>
+    <t>CN102521778A  20111208</t>
+  </si>
+  <si>
+    <t>201110407040</t>
+  </si>
+  <si>
+    <t>CN20111407040 20111208</t>
+  </si>
+  <si>
+    <t>CN103078911A  20121227</t>
+  </si>
+  <si>
+    <t>201210580153</t>
+  </si>
+  <si>
+    <t>CN20121580153 20121227</t>
   </si>
   <si>
     <t>2012-12-27</t>
   </si>
   <si>
-    <t>103679960</t>
-  </si>
-  <si>
-    <t>CN20121325507</t>
+    <t>CN103679960A  20120906</t>
+  </si>
+  <si>
+    <t>201210325507</t>
+  </si>
+  <si>
+    <t>CN20121325507 20120906</t>
   </si>
   <si>
     <t>2012-09-06</t>
   </si>
   <si>
-    <t>102542645</t>
-  </si>
-  <si>
-    <t>CN2012110295</t>
+    <t>CN102542645A  20120113</t>
+  </si>
+  <si>
+    <t>201210010295</t>
+  </si>
+  <si>
+    <t>CN2012110295 20120113</t>
   </si>
   <si>
     <t>2012-01-13</t>
   </si>
   <si>
-    <t>103985204</t>
-  </si>
-  <si>
-    <t>CN20141185927</t>
+    <t>CN103985204A  20140505</t>
+  </si>
+  <si>
+    <t>2014-08-13</t>
+  </si>
+  <si>
+    <t>201410185927</t>
+  </si>
+  <si>
+    <t>CN20141185927 20140505</t>
   </si>
   <si>
     <t>2014-05-05</t>
   </si>
   <si>
-    <t>2015074416</t>
-  </si>
-  <si>
-    <t>WO2014CN80514</t>
+    <t>CN2015074416W  20140623</t>
+  </si>
+  <si>
+    <t>2015-05-28</t>
+  </si>
+  <si>
+    <t>2014080514</t>
+  </si>
+  <si>
+    <t>WO2014CN80514 20140623</t>
   </si>
   <si>
     <t>2014-06-23</t>
@@ -848,12 +1301,13 @@
     <col min="4" max="4" width="30.15234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="20.3203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="36.26171875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="29.96484375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="26.40234375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="33.36328125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="36.19140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="33.1484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="29.96484375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="26.49609375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="43.61328125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="36.19140625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="36.19140625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="33.00390625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="29.72265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -888,10 +1342,13 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -911,25 +1368,28 @@
         <v>4.23126133E8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -949,25 +1409,28 @@
         <v>4.38032035E8</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -987,25 +1450,28 @@
         <v>4.21869315E8</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -1025,25 +1491,28 @@
         <v>4.18067657E8</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6">
@@ -1063,25 +1532,28 @@
         <v>4.18069767E8</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7">
@@ -1101,25 +1573,28 @@
         <v>4.11517079E8</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8">
@@ -1139,25 +1614,28 @@
         <v>4.06247368E8</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9">
@@ -1177,25 +1655,28 @@
         <v>4.16564519E8</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10">
@@ -1215,25 +1696,28 @@
         <v>4.39568795E8</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -1253,25 +1737,28 @@
         <v>4.39569039E8</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L11" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12">
@@ -1291,25 +1778,28 @@
         <v>3.84434075E8</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="J12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13">
@@ -1329,25 +1819,28 @@
         <v>3.84502942E8</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="J13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -1367,25 +1860,28 @@
         <v>4.08748768E8</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L14" t="s">
-        <v>49</v>
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -1405,25 +1901,28 @@
         <v>4.16320589E8</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="J15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K15" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="M15" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16">
@@ -1443,25 +1942,28 @@
         <v>4.19040478E8</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="J16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K16" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L16" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="M16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="17">
@@ -1481,25 +1983,28 @@
         <v>4.2030526E8</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="J17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L17" t="s">
-        <v>58</v>
+        <v>19</v>
+      </c>
+      <c r="M17" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18">
@@ -1519,25 +2024,28 @@
         <v>4.37816203E8</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>19</v>
+      </c>
+      <c r="M18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19">
@@ -1557,25 +2065,28 @@
         <v>4.40346278E8</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L19" t="s">
-        <v>64</v>
+        <v>19</v>
+      </c>
+      <c r="M19" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -1595,25 +2106,28 @@
         <v>3.65418009E8</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="J20" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>67</v>
+        <v>19</v>
+      </c>
+      <c r="M20" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21">
@@ -1633,25 +2147,28 @@
         <v>4.17201656E8</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="J21" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L21" t="s">
-        <v>70</v>
+        <v>19</v>
+      </c>
+      <c r="M21" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="22">
@@ -1671,25 +2188,28 @@
         <v>3.63783676E8</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="H22" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="J22" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K22" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L22" t="s">
-        <v>73</v>
+        <v>19</v>
+      </c>
+      <c r="M22" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="23">
@@ -1709,25 +2229,28 @@
         <v>3.63783676E8</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="H23" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="J23" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K23" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L23" t="s">
-        <v>73</v>
+        <v>19</v>
+      </c>
+      <c r="M23" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="24">
@@ -1747,25 +2270,28 @@
         <v>4.06971348E8</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="H24" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="J24" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K24" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L24" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="M24" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="25">
@@ -1785,25 +2311,28 @@
         <v>4.16080416E8</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="J25" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K25" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L25" t="s">
-        <v>79</v>
+        <v>19</v>
+      </c>
+      <c r="M25" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="26">
@@ -1823,25 +2352,28 @@
         <v>4.1656423E8</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="J26" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K26" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L26" t="s">
-        <v>82</v>
+        <v>19</v>
+      </c>
+      <c r="M26" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="27">
@@ -1861,25 +2393,28 @@
         <v>3.53265278E8</v>
       </c>
       <c r="F27" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="H27" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="J27" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K27" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L27" t="s">
-        <v>85</v>
+        <v>19</v>
+      </c>
+      <c r="M27" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="28">
@@ -1899,25 +2434,28 @@
         <v>3.7505585E8</v>
       </c>
       <c r="F28" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="H28" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="I28" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="J28" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K28" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L28" t="s">
-        <v>88</v>
+        <v>19</v>
+      </c>
+      <c r="M28" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="29">
@@ -1937,25 +2475,28 @@
         <v>3.80035266E8</v>
       </c>
       <c r="F29" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>142</v>
       </c>
       <c r="H29" t="s">
-        <v>90</v>
+        <v>143</v>
       </c>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="J29" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K29" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L29" t="s">
-        <v>91</v>
+        <v>19</v>
+      </c>
+      <c r="M29" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="30">
@@ -1975,25 +2516,28 @@
         <v>3.80073846E8</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>142</v>
       </c>
       <c r="H30" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="J30" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K30" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L30" t="s">
-        <v>91</v>
+        <v>19</v>
+      </c>
+      <c r="M30" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="31">
@@ -2013,25 +2557,28 @@
         <v>3.80075929E8</v>
       </c>
       <c r="F31" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="H31" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="I31" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="J31" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K31" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L31" t="s">
-        <v>96</v>
+        <v>19</v>
+      </c>
+      <c r="M31" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="32">
@@ -2051,25 +2598,28 @@
         <v>3.80278975E8</v>
       </c>
       <c r="F32" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="H32" t="s">
-        <v>98</v>
+        <v>155</v>
       </c>
       <c r="I32" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="J32" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K32" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L32" t="s">
-        <v>99</v>
+        <v>19</v>
+      </c>
+      <c r="M32" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="33">
@@ -2089,25 +2639,28 @@
         <v>3.84461097E8</v>
       </c>
       <c r="F33" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
       <c r="H33" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="I33" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="J33" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K33" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L33" t="s">
-        <v>102</v>
+        <v>19</v>
+      </c>
+      <c r="M33" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="34">
@@ -2127,25 +2680,28 @@
         <v>4.10384013E8</v>
       </c>
       <c r="F34" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
       <c r="H34" t="s">
-        <v>104</v>
+        <v>165</v>
       </c>
       <c r="I34" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="J34" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K34" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L34" t="s">
-        <v>105</v>
+        <v>19</v>
+      </c>
+      <c r="M34" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="35">
@@ -2165,25 +2721,28 @@
         <v>4.10384015E8</v>
       </c>
       <c r="F35" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
       <c r="H35" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
       <c r="I35" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="J35" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K35" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L35" t="s">
-        <v>108</v>
+        <v>19</v>
+      </c>
+      <c r="M35" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="36">
@@ -2203,25 +2762,28 @@
         <v>4.13163522E8</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="H36" t="s">
-        <v>110</v>
+        <v>174</v>
       </c>
       <c r="I36" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="J36" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K36" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L36" t="s">
-        <v>111</v>
+        <v>19</v>
+      </c>
+      <c r="M36" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="37">
@@ -2241,25 +2803,28 @@
         <v>4.18808725E8</v>
       </c>
       <c r="F37" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="G37" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="H37" t="s">
-        <v>113</v>
+        <v>179</v>
       </c>
       <c r="I37" t="s">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="J37" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K37" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L37" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="M37" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="38">
@@ -2279,25 +2844,28 @@
         <v>3.81603953E8</v>
       </c>
       <c r="F38" t="s">
-        <v>114</v>
+        <v>181</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="H38" t="s">
-        <v>115</v>
+        <v>183</v>
       </c>
       <c r="I38" t="s">
-        <v>11</v>
+        <v>184</v>
       </c>
       <c r="J38" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K38" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L38" t="s">
-        <v>116</v>
+        <v>19</v>
+      </c>
+      <c r="M38" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="39">
@@ -2317,25 +2885,28 @@
         <v>3.84443623E8</v>
       </c>
       <c r="F39" t="s">
-        <v>117</v>
+        <v>186</v>
       </c>
       <c r="G39" t="s">
-        <v>11</v>
+        <v>187</v>
       </c>
       <c r="H39" t="s">
-        <v>118</v>
+        <v>188</v>
       </c>
       <c r="I39" t="s">
-        <v>11</v>
+        <v>189</v>
       </c>
       <c r="J39" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K39" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L39" t="s">
-        <v>119</v>
+        <v>19</v>
+      </c>
+      <c r="M39" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="40">
@@ -2355,25 +2926,28 @@
         <v>4.18807977E8</v>
       </c>
       <c r="F40" t="s">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="H40" t="s">
-        <v>121</v>
+        <v>192</v>
       </c>
       <c r="I40" t="s">
-        <v>11</v>
+        <v>193</v>
       </c>
       <c r="J40" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K40" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L40" t="s">
-        <v>122</v>
+        <v>19</v>
+      </c>
+      <c r="M40" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="41">
@@ -2393,25 +2967,28 @@
         <v>3.65835465E8</v>
       </c>
       <c r="F41" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="G41" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="H41" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
       <c r="I41" t="s">
-        <v>11</v>
+        <v>197</v>
       </c>
       <c r="J41" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K41" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L41" t="s">
-        <v>125</v>
+        <v>19</v>
+      </c>
+      <c r="M41" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="42">
@@ -2431,25 +3008,28 @@
         <v>4.05601631E8</v>
       </c>
       <c r="F42" t="s">
-        <v>126</v>
+        <v>199</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="H42" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="I42" t="s">
-        <v>11</v>
+        <v>202</v>
       </c>
       <c r="J42" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K42" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L42" t="s">
-        <v>128</v>
+        <v>19</v>
+      </c>
+      <c r="M42" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="43">
@@ -2469,25 +3049,28 @@
         <v>3.74890738E8</v>
       </c>
       <c r="F43" t="s">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c r="G43" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="H43" t="s">
-        <v>130</v>
+        <v>206</v>
       </c>
       <c r="I43" t="s">
-        <v>11</v>
+        <v>207</v>
       </c>
       <c r="J43" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K43" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L43" t="s">
-        <v>131</v>
+        <v>19</v>
+      </c>
+      <c r="M43" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="44">
@@ -2507,25 +3090,28 @@
         <v>4.21854295E8</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>209</v>
       </c>
       <c r="G44" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H44" t="s">
-        <v>133</v>
+        <v>210</v>
       </c>
       <c r="I44" t="s">
-        <v>11</v>
+        <v>211</v>
       </c>
       <c r="J44" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K44" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L44" t="s">
-        <v>134</v>
+        <v>19</v>
+      </c>
+      <c r="M44" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="45">
@@ -2545,25 +3131,28 @@
         <v>3.5300229E8</v>
       </c>
       <c r="F45" t="s">
-        <v>135</v>
+        <v>213</v>
       </c>
       <c r="G45" t="s">
-        <v>11</v>
+        <v>214</v>
       </c>
       <c r="H45" t="s">
-        <v>136</v>
+        <v>215</v>
       </c>
       <c r="I45" t="s">
-        <v>11</v>
+        <v>216</v>
       </c>
       <c r="J45" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K45" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L45" t="s">
-        <v>137</v>
+        <v>19</v>
+      </c>
+      <c r="M45" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="46">
@@ -2583,25 +3172,28 @@
         <v>3.79761525E8</v>
       </c>
       <c r="F46" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>219</v>
       </c>
       <c r="H46" t="s">
-        <v>139</v>
+        <v>220</v>
       </c>
       <c r="I46" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="J46" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
       <c r="K46" t="s">
-        <v>14</v>
+        <v>222</v>
       </c>
       <c r="L46" t="s">
-        <v>141</v>
+        <v>19</v>
+      </c>
+      <c r="M46" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="47">
@@ -2621,25 +3213,28 @@
         <v>3.84441809E8</v>
       </c>
       <c r="F47" t="s">
-        <v>142</v>
+        <v>224</v>
       </c>
       <c r="G47" t="s">
-        <v>11</v>
+        <v>187</v>
       </c>
       <c r="H47" t="s">
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="I47" t="s">
-        <v>11</v>
+        <v>226</v>
       </c>
       <c r="J47" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K47" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L47" t="s">
-        <v>144</v>
+        <v>19</v>
+      </c>
+      <c r="M47" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="48">
@@ -2659,25 +3254,28 @@
         <v>4.07669688E8</v>
       </c>
       <c r="F48" t="s">
-        <v>145</v>
+        <v>228</v>
       </c>
       <c r="G48" t="s">
-        <v>11</v>
+        <v>229</v>
       </c>
       <c r="H48" t="s">
-        <v>146</v>
+        <v>230</v>
       </c>
       <c r="I48" t="s">
-        <v>11</v>
+        <v>231</v>
       </c>
       <c r="J48" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K48" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L48" t="s">
-        <v>88</v>
+        <v>19</v>
+      </c>
+      <c r="M48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49">
@@ -2697,25 +3295,28 @@
         <v>4.1515437E8</v>
       </c>
       <c r="F49" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="G49" t="s">
-        <v>11</v>
+        <v>232</v>
       </c>
       <c r="H49" t="s">
-        <v>139</v>
+        <v>220</v>
       </c>
       <c r="I49" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="J49" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
       <c r="K49" t="s">
-        <v>14</v>
+        <v>222</v>
       </c>
       <c r="L49" t="s">
-        <v>141</v>
+        <v>19</v>
+      </c>
+      <c r="M49" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="50">
@@ -2735,25 +3336,28 @@
         <v>4.16564537E8</v>
       </c>
       <c r="F50" t="s">
-        <v>147</v>
+        <v>233</v>
       </c>
       <c r="G50" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="H50" t="s">
-        <v>148</v>
+        <v>234</v>
       </c>
       <c r="I50" t="s">
-        <v>11</v>
+        <v>235</v>
       </c>
       <c r="J50" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K50" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L50" t="s">
-        <v>149</v>
+        <v>19</v>
+      </c>
+      <c r="M50" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="51">
@@ -2773,25 +3377,28 @@
         <v>4.16989412E8</v>
       </c>
       <c r="F51" t="s">
-        <v>150</v>
+        <v>237</v>
       </c>
       <c r="G51" t="s">
-        <v>11</v>
+        <v>238</v>
       </c>
       <c r="H51" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="I51" t="s">
-        <v>11</v>
+        <v>240</v>
       </c>
       <c r="J51" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K51" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L51" t="s">
-        <v>79</v>
+        <v>19</v>
+      </c>
+      <c r="M51" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="52">
@@ -2811,25 +3418,28 @@
         <v>3.41758296E8</v>
       </c>
       <c r="F52" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="G52" t="s">
-        <v>11</v>
+        <v>242</v>
       </c>
       <c r="H52" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="I52" t="s">
-        <v>11</v>
+        <v>244</v>
       </c>
       <c r="J52" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K52" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L52" t="s">
-        <v>154</v>
+        <v>19</v>
+      </c>
+      <c r="M52" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="53">
@@ -2849,25 +3459,28 @@
         <v>3.65836212E8</v>
       </c>
       <c r="F53" t="s">
-        <v>155</v>
+        <v>246</v>
       </c>
       <c r="G53" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="H53" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="I53" t="s">
-        <v>11</v>
+        <v>248</v>
       </c>
       <c r="J53" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K53" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L53" t="s">
-        <v>157</v>
+        <v>19</v>
+      </c>
+      <c r="M53" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="54">
@@ -2887,25 +3500,28 @@
         <v>4.14727847E8</v>
       </c>
       <c r="F54" t="s">
-        <v>158</v>
+        <v>250</v>
       </c>
       <c r="G54" t="s">
-        <v>11</v>
+        <v>251</v>
       </c>
       <c r="H54" t="s">
-        <v>159</v>
+        <v>252</v>
       </c>
       <c r="I54" t="s">
-        <v>11</v>
+        <v>253</v>
       </c>
       <c r="J54" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K54" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L54" t="s">
-        <v>160</v>
+        <v>19</v>
+      </c>
+      <c r="M54" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="55">
@@ -2925,25 +3541,28 @@
         <v>3.36658357E8</v>
       </c>
       <c r="F55" t="s">
-        <v>161</v>
+        <v>255</v>
       </c>
       <c r="G55" t="s">
-        <v>11</v>
+        <v>256</v>
       </c>
       <c r="H55" t="s">
-        <v>162</v>
+        <v>257</v>
       </c>
       <c r="I55" t="s">
-        <v>11</v>
+        <v>258</v>
       </c>
       <c r="J55" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K55" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L55" t="s">
-        <v>163</v>
+        <v>19</v>
+      </c>
+      <c r="M55" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="56">
@@ -2963,25 +3582,28 @@
         <v>4.12306752E8</v>
       </c>
       <c r="F56" t="s">
-        <v>164</v>
+        <v>260</v>
       </c>
       <c r="G56" t="s">
-        <v>11</v>
+        <v>261</v>
       </c>
       <c r="H56" t="s">
-        <v>165</v>
+        <v>262</v>
       </c>
       <c r="I56" t="s">
-        <v>11</v>
+        <v>263</v>
       </c>
       <c r="J56" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K56" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L56" t="s">
-        <v>166</v>
+        <v>19</v>
+      </c>
+      <c r="M56" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="57">
@@ -3001,25 +3623,28 @@
         <v>3.7574279E8</v>
       </c>
       <c r="F57" t="s">
-        <v>167</v>
+        <v>265</v>
       </c>
       <c r="G57" t="s">
-        <v>11</v>
+        <v>266</v>
       </c>
       <c r="H57" t="s">
-        <v>168</v>
+        <v>267</v>
       </c>
       <c r="I57" t="s">
-        <v>11</v>
+        <v>268</v>
       </c>
       <c r="J57" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K57" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L57" t="s">
-        <v>169</v>
+        <v>19</v>
+      </c>
+      <c r="M57" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="58">
@@ -3039,25 +3664,28 @@
         <v>4.05608703E8</v>
       </c>
       <c r="F58" t="s">
-        <v>170</v>
+        <v>270</v>
       </c>
       <c r="G58" t="s">
-        <v>11</v>
+        <v>271</v>
       </c>
       <c r="H58" t="s">
-        <v>171</v>
+        <v>272</v>
       </c>
       <c r="I58" t="s">
-        <v>11</v>
+        <v>273</v>
       </c>
       <c r="J58" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K58" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L58" t="s">
-        <v>172</v>
+        <v>19</v>
+      </c>
+      <c r="M58" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="59">
@@ -3077,25 +3705,28 @@
         <v>4.25429398E8</v>
       </c>
       <c r="F59" t="s">
-        <v>173</v>
+        <v>275</v>
       </c>
       <c r="G59" t="s">
-        <v>11</v>
+        <v>276</v>
       </c>
       <c r="H59" t="s">
-        <v>174</v>
+        <v>277</v>
       </c>
       <c r="I59" t="s">
-        <v>11</v>
+        <v>278</v>
       </c>
       <c r="J59" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K59" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L59" t="s">
-        <v>175</v>
+        <v>19</v>
+      </c>
+      <c r="M59" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="60">
@@ -3115,25 +3746,28 @@
         <v>3.36768E8</v>
       </c>
       <c r="F60" t="s">
-        <v>176</v>
+        <v>280</v>
       </c>
       <c r="G60" t="s">
-        <v>11</v>
+        <v>281</v>
       </c>
       <c r="H60" t="s">
-        <v>177</v>
+        <v>282</v>
       </c>
       <c r="I60" t="s">
-        <v>11</v>
+        <v>283</v>
       </c>
       <c r="J60" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K60" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L60" t="s">
-        <v>178</v>
+        <v>19</v>
+      </c>
+      <c r="M60" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="61">
@@ -3153,25 +3787,28 @@
         <v>4.40864114E8</v>
       </c>
       <c r="F61" t="s">
-        <v>179</v>
+        <v>285</v>
       </c>
       <c r="G61" t="s">
-        <v>11</v>
+        <v>286</v>
       </c>
       <c r="H61" t="s">
-        <v>180</v>
+        <v>287</v>
       </c>
       <c r="I61" t="s">
-        <v>11</v>
+        <v>288</v>
       </c>
       <c r="J61" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K61" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L61" t="s">
-        <v>181</v>
+        <v>19</v>
+      </c>
+      <c r="M61" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="62">
@@ -3191,25 +3828,28 @@
         <v>4.13638895E8</v>
       </c>
       <c r="F62" t="s">
-        <v>182</v>
+        <v>290</v>
       </c>
       <c r="G62" t="s">
-        <v>11</v>
+        <v>291</v>
       </c>
       <c r="H62" t="s">
-        <v>183</v>
+        <v>292</v>
       </c>
       <c r="I62" t="s">
-        <v>11</v>
+        <v>293</v>
       </c>
       <c r="J62" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K62" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L62" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="M62" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="63">
@@ -3229,25 +3869,28 @@
         <v>4.17468592E8</v>
       </c>
       <c r="F63" t="s">
-        <v>185</v>
+        <v>295</v>
       </c>
       <c r="G63" t="s">
-        <v>11</v>
+        <v>296</v>
       </c>
       <c r="H63" t="s">
-        <v>186</v>
+        <v>297</v>
       </c>
       <c r="I63" t="s">
-        <v>11</v>
+        <v>298</v>
       </c>
       <c r="J63" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K63" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L63" t="s">
-        <v>187</v>
+        <v>19</v>
+      </c>
+      <c r="M63" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="64">
@@ -3267,25 +3910,28 @@
         <v>4.19048591E8</v>
       </c>
       <c r="F64" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="G64" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="H64" t="s">
-        <v>189</v>
+        <v>301</v>
       </c>
       <c r="I64" t="s">
-        <v>11</v>
+        <v>302</v>
       </c>
       <c r="J64" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K64" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L64" t="s">
-        <v>190</v>
+        <v>19</v>
+      </c>
+      <c r="M64" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="65">
@@ -3305,25 +3951,28 @@
         <v>4.19048591E8</v>
       </c>
       <c r="F65" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="G65" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="H65" t="s">
-        <v>189</v>
+        <v>301</v>
       </c>
       <c r="I65" t="s">
-        <v>11</v>
+        <v>302</v>
       </c>
       <c r="J65" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K65" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L65" t="s">
-        <v>190</v>
+        <v>19</v>
+      </c>
+      <c r="M65" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="66">
@@ -3343,25 +3992,28 @@
         <v>4.05784597E8</v>
       </c>
       <c r="F66" t="s">
-        <v>191</v>
+        <v>303</v>
       </c>
       <c r="G66" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="H66" t="s">
-        <v>192</v>
+        <v>305</v>
       </c>
       <c r="I66" t="s">
-        <v>11</v>
+        <v>306</v>
       </c>
       <c r="J66" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K66" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L66" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="M66" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="67">
@@ -3381,25 +4033,28 @@
         <v>4.16368441E8</v>
       </c>
       <c r="F67" t="s">
-        <v>193</v>
+        <v>307</v>
       </c>
       <c r="G67" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="H67" t="s">
-        <v>194</v>
+        <v>308</v>
       </c>
       <c r="I67" t="s">
-        <v>11</v>
+        <v>309</v>
       </c>
       <c r="J67" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K67" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L67" t="s">
-        <v>195</v>
+        <v>19</v>
+      </c>
+      <c r="M67" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="68">
@@ -3419,25 +4074,28 @@
         <v>4.16815513E8</v>
       </c>
       <c r="F68" t="s">
-        <v>196</v>
+        <v>311</v>
       </c>
       <c r="G68" t="s">
-        <v>11</v>
+        <v>312</v>
       </c>
       <c r="H68" t="s">
-        <v>197</v>
+        <v>313</v>
       </c>
       <c r="I68" t="s">
-        <v>11</v>
+        <v>314</v>
       </c>
       <c r="J68" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K68" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L68" t="s">
-        <v>198</v>
+        <v>19</v>
+      </c>
+      <c r="M68" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="69">
@@ -3457,25 +4115,28 @@
         <v>2.77258962E8</v>
       </c>
       <c r="F69" t="s">
-        <v>199</v>
+        <v>316</v>
       </c>
       <c r="G69" t="s">
-        <v>11</v>
+        <v>317</v>
       </c>
       <c r="H69" t="s">
-        <v>200</v>
+        <v>318</v>
       </c>
       <c r="I69" t="s">
-        <v>11</v>
+        <v>319</v>
       </c>
       <c r="J69" t="s">
-        <v>13</v>
+        <v>320</v>
       </c>
       <c r="K69" t="s">
-        <v>201</v>
+        <v>18</v>
       </c>
       <c r="L69" t="s">
-        <v>202</v>
+        <v>321</v>
+      </c>
+      <c r="M69" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="70">
@@ -3495,25 +4156,28 @@
         <v>3.33967698E8</v>
       </c>
       <c r="F70" t="s">
-        <v>203</v>
+        <v>323</v>
       </c>
       <c r="G70" t="s">
-        <v>11</v>
+        <v>324</v>
       </c>
       <c r="H70" t="s">
-        <v>204</v>
+        <v>325</v>
       </c>
       <c r="I70" t="s">
-        <v>11</v>
+        <v>326</v>
       </c>
       <c r="J70" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K70" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L70" t="s">
-        <v>205</v>
+        <v>19</v>
+      </c>
+      <c r="M70" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="71">
@@ -3533,25 +4197,28 @@
         <v>4.05598338E8</v>
       </c>
       <c r="F71" t="s">
-        <v>206</v>
+        <v>328</v>
       </c>
       <c r="G71" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="H71" t="s">
-        <v>207</v>
+        <v>329</v>
       </c>
       <c r="I71" t="s">
-        <v>11</v>
+        <v>330</v>
       </c>
       <c r="J71" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K71" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L71" t="s">
-        <v>208</v>
+        <v>19</v>
+      </c>
+      <c r="M71" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="72">
@@ -3571,25 +4238,28 @@
         <v>3.52680521E8</v>
       </c>
       <c r="F72" t="s">
-        <v>209</v>
+        <v>332</v>
       </c>
       <c r="G72" t="s">
-        <v>11</v>
+        <v>333</v>
       </c>
       <c r="H72" t="s">
-        <v>210</v>
+        <v>334</v>
       </c>
       <c r="I72" t="s">
-        <v>11</v>
+        <v>335</v>
       </c>
       <c r="J72" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K72" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L72" t="s">
-        <v>211</v>
+        <v>19</v>
+      </c>
+      <c r="M72" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="73">
@@ -3609,25 +4279,28 @@
         <v>3.84434927E8</v>
       </c>
       <c r="F73" t="s">
-        <v>212</v>
+        <v>337</v>
       </c>
       <c r="G73" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="H73" t="s">
-        <v>213</v>
+        <v>338</v>
       </c>
       <c r="I73" t="s">
-        <v>11</v>
+        <v>339</v>
       </c>
       <c r="J73" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K73" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L73" t="s">
-        <v>214</v>
+        <v>19</v>
+      </c>
+      <c r="M73" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="74">
@@ -3647,25 +4320,28 @@
         <v>4.07665131E8</v>
       </c>
       <c r="F74" t="s">
-        <v>215</v>
+        <v>341</v>
       </c>
       <c r="G74" t="s">
-        <v>11</v>
+        <v>229</v>
       </c>
       <c r="H74" t="s">
-        <v>216</v>
+        <v>342</v>
       </c>
       <c r="I74" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="J74" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K74" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L74" t="s">
-        <v>217</v>
+        <v>19</v>
+      </c>
+      <c r="M74" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="75">
@@ -3685,25 +4361,28 @@
         <v>4.22599862E8</v>
       </c>
       <c r="F75" t="s">
-        <v>218</v>
+        <v>345</v>
       </c>
       <c r="G75" t="s">
-        <v>11</v>
+        <v>346</v>
       </c>
       <c r="H75" t="s">
-        <v>219</v>
+        <v>347</v>
       </c>
       <c r="I75" t="s">
-        <v>11</v>
+        <v>348</v>
       </c>
       <c r="J75" t="s">
-        <v>13</v>
+        <v>320</v>
       </c>
       <c r="K75" t="s">
-        <v>201</v>
+        <v>18</v>
       </c>
       <c r="L75" t="s">
-        <v>220</v>
+        <v>321</v>
+      </c>
+      <c r="M75" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="76">
@@ -3723,25 +4402,28 @@
         <v>3.81151747E8</v>
       </c>
       <c r="F76" t="s">
-        <v>221</v>
+        <v>350</v>
       </c>
       <c r="G76" t="s">
-        <v>11</v>
+        <v>351</v>
       </c>
       <c r="H76" t="s">
-        <v>222</v>
+        <v>352</v>
       </c>
       <c r="I76" t="s">
-        <v>11</v>
+        <v>353</v>
       </c>
       <c r="J76" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K76" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L76" t="s">
-        <v>223</v>
+        <v>19</v>
+      </c>
+      <c r="M76" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="77">
@@ -3761,25 +4443,28 @@
         <v>3.8162995E8</v>
       </c>
       <c r="F77" t="s">
-        <v>224</v>
+        <v>355</v>
       </c>
       <c r="G77" t="s">
-        <v>11</v>
+        <v>356</v>
       </c>
       <c r="H77" t="s">
-        <v>225</v>
+        <v>357</v>
       </c>
       <c r="I77" t="s">
-        <v>11</v>
+        <v>358</v>
       </c>
       <c r="J77" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K77" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L77" t="s">
-        <v>226</v>
+        <v>19</v>
+      </c>
+      <c r="M77" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="78">
@@ -3799,25 +4484,28 @@
         <v>4.0711782E8</v>
       </c>
       <c r="F78" t="s">
-        <v>227</v>
+        <v>360</v>
       </c>
       <c r="G78" t="s">
-        <v>11</v>
+        <v>361</v>
       </c>
       <c r="H78" t="s">
-        <v>228</v>
+        <v>362</v>
       </c>
       <c r="I78" t="s">
-        <v>11</v>
+        <v>363</v>
       </c>
       <c r="J78" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K78" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L78" t="s">
-        <v>229</v>
+        <v>19</v>
+      </c>
+      <c r="M78" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="79">
@@ -3837,25 +4525,28 @@
         <v>3.41975587E8</v>
       </c>
       <c r="F79" t="s">
-        <v>230</v>
+        <v>365</v>
       </c>
       <c r="G79" t="s">
-        <v>11</v>
+        <v>366</v>
       </c>
       <c r="H79" t="s">
-        <v>231</v>
+        <v>367</v>
       </c>
       <c r="I79" t="s">
-        <v>11</v>
+        <v>368</v>
       </c>
       <c r="J79" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K79" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L79" t="s">
-        <v>232</v>
+        <v>19</v>
+      </c>
+      <c r="M79" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="80">
@@ -3875,25 +4566,28 @@
         <v>3.65413218E8</v>
       </c>
       <c r="F80" t="s">
-        <v>233</v>
+        <v>370</v>
       </c>
       <c r="G80" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="H80" t="s">
-        <v>234</v>
+        <v>371</v>
       </c>
       <c r="I80" t="s">
-        <v>11</v>
+        <v>372</v>
       </c>
       <c r="J80" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K80" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L80" t="s">
-        <v>235</v>
+        <v>19</v>
+      </c>
+      <c r="M80" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="81">
@@ -3913,25 +4607,28 @@
         <v>3.65923468E8</v>
       </c>
       <c r="F81" t="s">
-        <v>236</v>
+        <v>374</v>
       </c>
       <c r="G81" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="H81" t="s">
-        <v>237</v>
+        <v>375</v>
       </c>
       <c r="I81" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
       <c r="J81" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K81" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L81" t="s">
-        <v>238</v>
+        <v>19</v>
+      </c>
+      <c r="M81" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="82">
@@ -3951,25 +4648,28 @@
         <v>4.08982321E8</v>
       </c>
       <c r="F82" t="s">
-        <v>239</v>
+        <v>378</v>
       </c>
       <c r="G82" t="s">
-        <v>11</v>
+        <v>379</v>
       </c>
       <c r="H82" t="s">
-        <v>240</v>
+        <v>380</v>
       </c>
       <c r="I82" t="s">
-        <v>11</v>
+        <v>381</v>
       </c>
       <c r="J82" t="s">
-        <v>13</v>
+        <v>320</v>
       </c>
       <c r="K82" t="s">
-        <v>201</v>
+        <v>18</v>
       </c>
       <c r="L82" t="s">
-        <v>172</v>
+        <v>321</v>
+      </c>
+      <c r="M82" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="83">
@@ -3989,25 +4689,28 @@
         <v>3.34788937E8</v>
       </c>
       <c r="F83" t="s">
-        <v>241</v>
+        <v>382</v>
       </c>
       <c r="G83" t="s">
-        <v>11</v>
+        <v>383</v>
       </c>
       <c r="H83" t="s">
-        <v>242</v>
+        <v>384</v>
       </c>
       <c r="I83" t="s">
-        <v>11</v>
+        <v>385</v>
       </c>
       <c r="J83" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K83" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L83" t="s">
-        <v>163</v>
+        <v>19</v>
+      </c>
+      <c r="M83" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="84">
@@ -4027,25 +4730,28 @@
         <v>3.65767908E8</v>
       </c>
       <c r="F84" t="s">
-        <v>243</v>
+        <v>386</v>
       </c>
       <c r="G84" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="H84" t="s">
-        <v>244</v>
+        <v>387</v>
       </c>
       <c r="I84" t="s">
-        <v>11</v>
+        <v>388</v>
       </c>
       <c r="J84" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K84" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L84" t="s">
-        <v>217</v>
+        <v>19</v>
+      </c>
+      <c r="M84" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="85">
@@ -4065,25 +4771,28 @@
         <v>4.05598338E8</v>
       </c>
       <c r="F85" t="s">
-        <v>206</v>
+        <v>328</v>
       </c>
       <c r="G85" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="H85" t="s">
-        <v>207</v>
+        <v>329</v>
       </c>
       <c r="I85" t="s">
-        <v>11</v>
+        <v>330</v>
       </c>
       <c r="J85" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K85" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L85" t="s">
-        <v>208</v>
+        <v>19</v>
+      </c>
+      <c r="M85" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="86">
@@ -4103,25 +4812,28 @@
         <v>4.06241522E8</v>
       </c>
       <c r="F86" t="s">
-        <v>245</v>
+        <v>389</v>
       </c>
       <c r="G86" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="H86" t="s">
-        <v>246</v>
+        <v>390</v>
       </c>
       <c r="I86" t="s">
-        <v>11</v>
+        <v>391</v>
       </c>
       <c r="J86" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K86" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L86" t="s">
-        <v>247</v>
+        <v>19</v>
+      </c>
+      <c r="M86" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="87">
@@ -4141,25 +4853,28 @@
         <v>4.16358849E8</v>
       </c>
       <c r="F87" t="s">
-        <v>248</v>
+        <v>393</v>
       </c>
       <c r="G87" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="H87" t="s">
-        <v>249</v>
+        <v>394</v>
       </c>
       <c r="I87" t="s">
-        <v>11</v>
+        <v>395</v>
       </c>
       <c r="J87" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K87" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L87" t="s">
-        <v>250</v>
+        <v>19</v>
+      </c>
+      <c r="M87" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="88">
@@ -4179,25 +4894,28 @@
         <v>3.65786643E8</v>
       </c>
       <c r="F88" t="s">
-        <v>251</v>
+        <v>397</v>
       </c>
       <c r="G88" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="H88" t="s">
-        <v>252</v>
+        <v>398</v>
       </c>
       <c r="I88" t="s">
-        <v>11</v>
+        <v>399</v>
       </c>
       <c r="J88" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K88" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L88" t="s">
-        <v>253</v>
+        <v>19</v>
+      </c>
+      <c r="M88" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="89">
@@ -4217,25 +4935,28 @@
         <v>4.20823414E8</v>
       </c>
       <c r="F89" t="s">
-        <v>254</v>
+        <v>401</v>
       </c>
       <c r="G89" t="s">
-        <v>11</v>
+        <v>402</v>
       </c>
       <c r="H89" t="s">
-        <v>255</v>
+        <v>403</v>
       </c>
       <c r="I89" t="s">
-        <v>11</v>
+        <v>404</v>
       </c>
       <c r="J89" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K89" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L89" t="s">
-        <v>256</v>
+        <v>19</v>
+      </c>
+      <c r="M89" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="90">
@@ -4255,25 +4976,28 @@
         <v>4.40603601E8</v>
       </c>
       <c r="F90" t="s">
-        <v>257</v>
+        <v>406</v>
       </c>
       <c r="G90" t="s">
-        <v>11</v>
+        <v>407</v>
       </c>
       <c r="H90" t="s">
-        <v>258</v>
+        <v>408</v>
       </c>
       <c r="I90" t="s">
-        <v>11</v>
+        <v>409</v>
       </c>
       <c r="J90" t="s">
-        <v>13</v>
+        <v>320</v>
       </c>
       <c r="K90" t="s">
-        <v>201</v>
+        <v>18</v>
       </c>
       <c r="L90" t="s">
-        <v>259</v>
+        <v>321</v>
+      </c>
+      <c r="M90" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added docdb family id
</commit_message>
<xml_diff>
--- a/citations.xlsx
+++ b/citations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="412">
   <si>
     <t>RAP - Citation ID</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>EPO - Citing Application Number</t>
+  </si>
+  <si>
+    <t>EPO - Citing Application DOCDB Family ID</t>
   </si>
   <si>
     <t>EPO - Citing Priority Number</t>
@@ -1303,11 +1306,12 @@
     <col min="6" max="6" width="36.26171875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="33.1484375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="29.96484375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="26.49609375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="43.61328125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.19140625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="33.00390625" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="29.72265625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="37.87890625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="26.49609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="43.61328125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="36.19140625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="33.00390625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="29.72265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1350,6 +1354,9 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1368,16 +1375,16 @@
         <v>4.23126133E8</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
         <v>16</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.176666E7</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
@@ -1390,6 +1397,9 @@
       </c>
       <c r="M2" t="s">
         <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -1409,19 +1419,19 @@
         <v>4.38032035E8</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
         <v>24</v>
       </c>
+      <c r="I3" t="n">
+        <v>5.2639094E7</v>
+      </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
         <v>18</v>
@@ -1430,7 +1440,10 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -1450,19 +1463,19 @@
         <v>4.21869315E8</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
         <v>29</v>
       </c>
+      <c r="I4" t="n">
+        <v>5.1504463E7</v>
+      </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>
@@ -1471,7 +1484,10 @@
         <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -1491,19 +1507,19 @@
         <v>4.18067657E8</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
         <v>34</v>
       </c>
+      <c r="I5" t="n">
+        <v>5.0699512E7</v>
+      </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
@@ -1512,7 +1528,10 @@
         <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6">
@@ -1532,19 +1551,19 @@
         <v>4.18069767E8</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" t="s">
         <v>38</v>
       </c>
+      <c r="I6" t="n">
+        <v>5.0700418E7</v>
+      </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
         <v>18</v>
@@ -1553,7 +1572,10 @@
         <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -1573,19 +1595,19 @@
         <v>4.11517079E8</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" t="s">
         <v>43</v>
       </c>
+      <c r="I7" t="n">
+        <v>4.9361461E7</v>
+      </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
@@ -1594,7 +1616,10 @@
         <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
+        <v>20</v>
+      </c>
+      <c r="N7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8">
@@ -1614,19 +1639,19 @@
         <v>4.06247368E8</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" t="s">
         <v>48</v>
       </c>
+      <c r="I8" t="n">
+        <v>4.8149313E7</v>
+      </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s">
         <v>18</v>
@@ -1635,7 +1660,10 @@
         <v>19</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9">
@@ -1655,19 +1683,19 @@
         <v>4.16564519E8</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" t="s">
         <v>53</v>
       </c>
+      <c r="I9" t="n">
+        <v>5.0354745E7</v>
+      </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="K9" t="s">
         <v>18</v>
@@ -1676,7 +1704,10 @@
         <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10">
@@ -1696,19 +1727,19 @@
         <v>4.39568795E8</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
         <v>58</v>
       </c>
+      <c r="I10" t="n">
+        <v>5.2967872E7</v>
+      </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="K10" t="s">
         <v>18</v>
@@ -1717,7 +1748,10 @@
         <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>20</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -1737,28 +1771,31 @@
         <v>4.39569039E8</v>
       </c>
       <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" t="n">
+        <v>5.2967942E7</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
         <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12">
@@ -1778,19 +1815,19 @@
         <v>3.84434075E8</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" t="s">
         <v>66</v>
       </c>
+      <c r="I12" t="n">
+        <v>4.7198294E7</v>
+      </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
@@ -1799,7 +1836,10 @@
         <v>19</v>
       </c>
       <c r="M12" t="s">
-        <v>67</v>
+        <v>20</v>
+      </c>
+      <c r="N12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -1819,19 +1859,19 @@
         <v>3.84502942E8</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" t="s">
         <v>71</v>
       </c>
+      <c r="I13" t="n">
+        <v>4.7569747E7</v>
+      </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
@@ -1840,7 +1880,10 @@
         <v>19</v>
       </c>
       <c r="M13" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
@@ -1860,19 +1903,19 @@
         <v>4.08748768E8</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
-      </c>
-      <c r="I14" t="s">
         <v>75</v>
       </c>
+      <c r="I14" t="n">
+        <v>4.8715614E7</v>
+      </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="K14" t="s">
         <v>18</v>
@@ -1881,7 +1924,10 @@
         <v>19</v>
       </c>
       <c r="M14" t="s">
-        <v>76</v>
+        <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15">
@@ -1901,19 +1947,19 @@
         <v>4.16320589E8</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" t="s">
         <v>80</v>
       </c>
+      <c r="I15" t="n">
+        <v>5.030019E7</v>
+      </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="K15" t="s">
         <v>18</v>
@@ -1922,7 +1968,10 @@
         <v>19</v>
       </c>
       <c r="M15" t="s">
-        <v>81</v>
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -1942,19 +1991,19 @@
         <v>4.19040478E8</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" t="s">
         <v>85</v>
       </c>
+      <c r="I16" t="n">
+        <v>5.0902485E7</v>
+      </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="K16" t="s">
         <v>18</v>
@@ -1963,7 +2012,10 @@
         <v>19</v>
       </c>
       <c r="M16" t="s">
-        <v>86</v>
+        <v>20</v>
+      </c>
+      <c r="N16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17">
@@ -1983,19 +2035,19 @@
         <v>4.2030526E8</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" t="s">
         <v>90</v>
       </c>
+      <c r="I17" t="n">
+        <v>5.1183211E7</v>
+      </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="K17" t="s">
         <v>18</v>
@@ -2004,7 +2056,10 @@
         <v>19</v>
       </c>
       <c r="M17" t="s">
-        <v>91</v>
+        <v>20</v>
+      </c>
+      <c r="N17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18">
@@ -2024,19 +2079,19 @@
         <v>4.37816203E8</v>
       </c>
       <c r="F18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H18" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" t="s">
         <v>95</v>
       </c>
+      <c r="I18" t="n">
+        <v>5.2611515E7</v>
+      </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="K18" t="s">
         <v>18</v>
@@ -2045,7 +2100,10 @@
         <v>19</v>
       </c>
       <c r="M18" t="s">
-        <v>96</v>
+        <v>20</v>
+      </c>
+      <c r="N18" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="19">
@@ -2065,19 +2123,19 @@
         <v>4.40346278E8</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" t="s">
         <v>100</v>
       </c>
+      <c r="I19" t="n">
+        <v>5.3116229E7</v>
+      </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -2086,7 +2144,10 @@
         <v>19</v>
       </c>
       <c r="M19" t="s">
-        <v>101</v>
+        <v>20</v>
+      </c>
+      <c r="N19" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20">
@@ -2106,19 +2167,19 @@
         <v>3.65418009E8</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H20" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" t="s">
         <v>105</v>
       </c>
+      <c r="I20" t="n">
+        <v>4.6188937E7</v>
+      </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="K20" t="s">
         <v>18</v>
@@ -2127,7 +2188,10 @@
         <v>19</v>
       </c>
       <c r="M20" t="s">
-        <v>106</v>
+        <v>20</v>
+      </c>
+      <c r="N20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="21">
@@ -2147,19 +2211,19 @@
         <v>4.17201656E8</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H21" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" t="s">
         <v>110</v>
       </c>
+      <c r="I21" t="n">
+        <v>5.0504522E7</v>
+      </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="K21" t="s">
         <v>18</v>
@@ -2168,7 +2232,10 @@
         <v>19</v>
       </c>
       <c r="M21" t="s">
-        <v>111</v>
+        <v>20</v>
+      </c>
+      <c r="N21" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22">
@@ -2188,19 +2255,19 @@
         <v>3.63783676E8</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" t="s">
         <v>115</v>
       </c>
+      <c r="I22" t="n">
+        <v>4.5959885E7</v>
+      </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
@@ -2209,7 +2276,10 @@
         <v>19</v>
       </c>
       <c r="M22" t="s">
-        <v>116</v>
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="23">
@@ -2229,19 +2299,19 @@
         <v>3.63783676E8</v>
       </c>
       <c r="F23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H23" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" t="s">
         <v>115</v>
       </c>
+      <c r="I23" t="n">
+        <v>4.5959885E7</v>
+      </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="K23" t="s">
         <v>18</v>
@@ -2250,7 +2320,10 @@
         <v>19</v>
       </c>
       <c r="M23" t="s">
-        <v>116</v>
+        <v>20</v>
+      </c>
+      <c r="N23" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="24">
@@ -2270,19 +2343,19 @@
         <v>4.06971348E8</v>
       </c>
       <c r="F24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H24" t="s">
-        <v>119</v>
-      </c>
-      <c r="I24" t="s">
         <v>120</v>
       </c>
+      <c r="I24" t="n">
+        <v>4.8413815E7</v>
+      </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="K24" t="s">
         <v>18</v>
@@ -2291,7 +2364,10 @@
         <v>19</v>
       </c>
       <c r="M24" t="s">
-        <v>121</v>
+        <v>20</v>
+      </c>
+      <c r="N24" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="25">
@@ -2311,19 +2387,19 @@
         <v>4.16080416E8</v>
       </c>
       <c r="F25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H25" t="s">
-        <v>124</v>
-      </c>
-      <c r="I25" t="s">
         <v>125</v>
       </c>
+      <c r="I25" t="n">
+        <v>5.0249872E7</v>
+      </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="K25" t="s">
         <v>18</v>
@@ -2332,7 +2408,10 @@
         <v>19</v>
       </c>
       <c r="M25" t="s">
-        <v>126</v>
+        <v>20</v>
+      </c>
+      <c r="N25" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="26">
@@ -2352,19 +2431,19 @@
         <v>4.1656423E8</v>
       </c>
       <c r="F26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H26" t="s">
-        <v>128</v>
-      </c>
-      <c r="I26" t="s">
         <v>129</v>
       </c>
+      <c r="I26" t="n">
+        <v>5.0354613E7</v>
+      </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -2373,7 +2452,10 @@
         <v>19</v>
       </c>
       <c r="M26" t="s">
-        <v>130</v>
+        <v>20</v>
+      </c>
+      <c r="N26" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="27">
@@ -2393,19 +2475,19 @@
         <v>3.53265278E8</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H27" t="s">
-        <v>133</v>
-      </c>
-      <c r="I27" t="s">
         <v>134</v>
       </c>
+      <c r="I27" t="n">
+        <v>4.5860248E7</v>
+      </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="K27" t="s">
         <v>18</v>
@@ -2414,7 +2496,10 @@
         <v>19</v>
       </c>
       <c r="M27" t="s">
-        <v>135</v>
+        <v>20</v>
+      </c>
+      <c r="N27" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="28">
@@ -2434,19 +2519,19 @@
         <v>3.7505585E8</v>
       </c>
       <c r="F28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H28" t="s">
-        <v>138</v>
-      </c>
-      <c r="I28" t="s">
         <v>139</v>
       </c>
+      <c r="I28" t="n">
+        <v>4.6289807E7</v>
+      </c>
       <c r="J28" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="K28" t="s">
         <v>18</v>
@@ -2455,7 +2540,10 @@
         <v>19</v>
       </c>
       <c r="M28" t="s">
-        <v>140</v>
+        <v>20</v>
+      </c>
+      <c r="N28" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="29">
@@ -2475,19 +2563,19 @@
         <v>3.80035266E8</v>
       </c>
       <c r="F29" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H29" t="s">
-        <v>143</v>
-      </c>
-      <c r="I29" t="s">
         <v>144</v>
       </c>
+      <c r="I29" t="n">
+        <v>4.689359E7</v>
+      </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -2496,7 +2584,10 @@
         <v>19</v>
       </c>
       <c r="M29" t="s">
-        <v>145</v>
+        <v>20</v>
+      </c>
+      <c r="N29" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30">
@@ -2516,28 +2607,31 @@
         <v>3.80073846E8</v>
       </c>
       <c r="F30" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" t="s">
+        <v>148</v>
+      </c>
+      <c r="I30" t="n">
+        <v>4.6893592E7</v>
+      </c>
+      <c r="J30" t="s">
+        <v>149</v>
+      </c>
+      <c r="K30" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" t="s">
+        <v>20</v>
+      </c>
+      <c r="N30" t="s">
         <v>146</v>
-      </c>
-      <c r="G30" t="s">
-        <v>142</v>
-      </c>
-      <c r="H30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I30" t="s">
-        <v>148</v>
-      </c>
-      <c r="J30" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" t="s">
-        <v>18</v>
-      </c>
-      <c r="L30" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="31">
@@ -2557,19 +2651,19 @@
         <v>3.80075929E8</v>
       </c>
       <c r="F31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H31" t="s">
-        <v>151</v>
-      </c>
-      <c r="I31" t="s">
         <v>152</v>
       </c>
+      <c r="I31" t="n">
+        <v>4.6811254E7</v>
+      </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>153</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>
@@ -2578,7 +2672,10 @@
         <v>19</v>
       </c>
       <c r="M31" t="s">
-        <v>153</v>
+        <v>20</v>
+      </c>
+      <c r="N31" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32">
@@ -2598,19 +2695,19 @@
         <v>3.80278975E8</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H32" t="s">
-        <v>155</v>
-      </c>
-      <c r="I32" t="s">
         <v>156</v>
       </c>
+      <c r="I32" t="n">
+        <v>4.6811217E7</v>
+      </c>
       <c r="J32" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="K32" t="s">
         <v>18</v>
@@ -2619,7 +2716,10 @@
         <v>19</v>
       </c>
       <c r="M32" t="s">
-        <v>157</v>
+        <v>20</v>
+      </c>
+      <c r="N32" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="33">
@@ -2639,19 +2739,19 @@
         <v>3.84461097E8</v>
       </c>
       <c r="F33" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G33" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H33" t="s">
-        <v>160</v>
-      </c>
-      <c r="I33" t="s">
         <v>161</v>
       </c>
+      <c r="I33" t="n">
+        <v>4.7329551E7</v>
+      </c>
       <c r="J33" t="s">
-        <v>17</v>
+        <v>162</v>
       </c>
       <c r="K33" t="s">
         <v>18</v>
@@ -2660,7 +2760,10 @@
         <v>19</v>
       </c>
       <c r="M33" t="s">
-        <v>162</v>
+        <v>20</v>
+      </c>
+      <c r="N33" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="34">
@@ -2680,19 +2783,19 @@
         <v>4.10384013E8</v>
       </c>
       <c r="F34" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H34" t="s">
-        <v>165</v>
-      </c>
-      <c r="I34" t="s">
         <v>166</v>
       </c>
+      <c r="I34" t="n">
+        <v>4.9132785E7</v>
+      </c>
       <c r="J34" t="s">
-        <v>17</v>
+        <v>167</v>
       </c>
       <c r="K34" t="s">
         <v>18</v>
@@ -2701,7 +2804,10 @@
         <v>19</v>
       </c>
       <c r="M34" t="s">
-        <v>167</v>
+        <v>20</v>
+      </c>
+      <c r="N34" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="35">
@@ -2721,19 +2827,19 @@
         <v>4.10384015E8</v>
       </c>
       <c r="F35" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G35" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H35" t="s">
-        <v>169</v>
-      </c>
-      <c r="I35" t="s">
         <v>170</v>
       </c>
+      <c r="I35" t="n">
+        <v>4.9132786E7</v>
+      </c>
       <c r="J35" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="K35" t="s">
         <v>18</v>
@@ -2742,7 +2848,10 @@
         <v>19</v>
       </c>
       <c r="M35" t="s">
-        <v>171</v>
+        <v>20</v>
+      </c>
+      <c r="N35" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="36">
@@ -2762,19 +2871,19 @@
         <v>4.13163522E8</v>
       </c>
       <c r="F36" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G36" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H36" t="s">
-        <v>174</v>
-      </c>
-      <c r="I36" t="s">
         <v>175</v>
       </c>
+      <c r="I36" t="n">
+        <v>4.9691875E7</v>
+      </c>
       <c r="J36" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="K36" t="s">
         <v>18</v>
@@ -2783,7 +2892,10 @@
         <v>19</v>
       </c>
       <c r="M36" t="s">
-        <v>176</v>
+        <v>20</v>
+      </c>
+      <c r="N36" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="37">
@@ -2803,19 +2915,19 @@
         <v>4.18808725E8</v>
       </c>
       <c r="F37" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G37" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H37" t="s">
-        <v>179</v>
-      </c>
-      <c r="I37" t="s">
         <v>180</v>
       </c>
+      <c r="I37" t="n">
+        <v>5.0859177E7</v>
+      </c>
       <c r="J37" t="s">
-        <v>17</v>
+        <v>181</v>
       </c>
       <c r="K37" t="s">
         <v>18</v>
@@ -2824,7 +2936,10 @@
         <v>19</v>
       </c>
       <c r="M37" t="s">
-        <v>86</v>
+        <v>20</v>
+      </c>
+      <c r="N37" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="38">
@@ -2844,19 +2959,19 @@
         <v>3.81603953E8</v>
       </c>
       <c r="F38" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G38" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H38" t="s">
-        <v>183</v>
-      </c>
-      <c r="I38" t="s">
         <v>184</v>
       </c>
+      <c r="I38" t="n">
+        <v>4.6990136E7</v>
+      </c>
       <c r="J38" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="K38" t="s">
         <v>18</v>
@@ -2865,7 +2980,10 @@
         <v>19</v>
       </c>
       <c r="M38" t="s">
-        <v>185</v>
+        <v>20</v>
+      </c>
+      <c r="N38" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="39">
@@ -2885,19 +3003,19 @@
         <v>3.84443623E8</v>
       </c>
       <c r="F39" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G39" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H39" t="s">
-        <v>188</v>
-      </c>
-      <c r="I39" t="s">
         <v>189</v>
       </c>
+      <c r="I39" t="n">
+        <v>4.7232547E7</v>
+      </c>
       <c r="J39" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="K39" t="s">
         <v>18</v>
@@ -2906,7 +3024,10 @@
         <v>19</v>
       </c>
       <c r="M39" t="s">
-        <v>190</v>
+        <v>20</v>
+      </c>
+      <c r="N39" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="40">
@@ -2926,19 +3047,19 @@
         <v>4.18807977E8</v>
       </c>
       <c r="F40" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G40" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H40" t="s">
-        <v>192</v>
-      </c>
-      <c r="I40" t="s">
         <v>193</v>
       </c>
+      <c r="I40" t="n">
+        <v>5.0858875E7</v>
+      </c>
       <c r="J40" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="K40" t="s">
         <v>18</v>
@@ -2947,7 +3068,10 @@
         <v>19</v>
       </c>
       <c r="M40" t="s">
-        <v>194</v>
+        <v>20</v>
+      </c>
+      <c r="N40" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="41">
@@ -2967,19 +3091,19 @@
         <v>3.65835465E8</v>
       </c>
       <c r="F41" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H41" t="s">
-        <v>196</v>
-      </c>
-      <c r="I41" t="s">
         <v>197</v>
       </c>
+      <c r="I41" t="n">
+        <v>4.6294477E7</v>
+      </c>
       <c r="J41" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="K41" t="s">
         <v>18</v>
@@ -2988,7 +3112,10 @@
         <v>19</v>
       </c>
       <c r="M41" t="s">
-        <v>198</v>
+        <v>20</v>
+      </c>
+      <c r="N41" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="42">
@@ -3008,19 +3135,19 @@
         <v>4.05601631E8</v>
       </c>
       <c r="F42" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G42" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H42" t="s">
-        <v>201</v>
-      </c>
-      <c r="I42" t="s">
         <v>202</v>
       </c>
+      <c r="I42" t="n">
+        <v>4.7760604E7</v>
+      </c>
       <c r="J42" t="s">
-        <v>17</v>
+        <v>203</v>
       </c>
       <c r="K42" t="s">
         <v>18</v>
@@ -3029,7 +3156,10 @@
         <v>19</v>
       </c>
       <c r="M42" t="s">
-        <v>203</v>
+        <v>20</v>
+      </c>
+      <c r="N42" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="43">
@@ -3049,19 +3179,19 @@
         <v>3.74890738E8</v>
       </c>
       <c r="F43" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G43" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H43" t="s">
-        <v>206</v>
-      </c>
-      <c r="I43" t="s">
         <v>207</v>
       </c>
+      <c r="I43" t="n">
+        <v>4.6338113E7</v>
+      </c>
       <c r="J43" t="s">
-        <v>17</v>
+        <v>208</v>
       </c>
       <c r="K43" t="s">
         <v>18</v>
@@ -3070,7 +3200,10 @@
         <v>19</v>
       </c>
       <c r="M43" t="s">
-        <v>208</v>
+        <v>20</v>
+      </c>
+      <c r="N43" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="44">
@@ -3090,19 +3223,19 @@
         <v>4.21854295E8</v>
       </c>
       <c r="F44" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H44" t="s">
-        <v>210</v>
-      </c>
-      <c r="I44" t="s">
         <v>211</v>
       </c>
+      <c r="I44" t="n">
+        <v>5.1498007E7</v>
+      </c>
       <c r="J44" t="s">
-        <v>17</v>
+        <v>212</v>
       </c>
       <c r="K44" t="s">
         <v>18</v>
@@ -3111,7 +3244,10 @@
         <v>19</v>
       </c>
       <c r="M44" t="s">
-        <v>212</v>
+        <v>20</v>
+      </c>
+      <c r="N44" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="45">
@@ -3131,19 +3267,19 @@
         <v>3.5300229E8</v>
       </c>
       <c r="F45" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G45" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H45" t="s">
-        <v>215</v>
-      </c>
-      <c r="I45" t="s">
         <v>216</v>
       </c>
+      <c r="I45" t="n">
+        <v>4.5821257E7</v>
+      </c>
       <c r="J45" t="s">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="K45" t="s">
         <v>18</v>
@@ -3152,7 +3288,10 @@
         <v>19</v>
       </c>
       <c r="M45" t="s">
-        <v>217</v>
+        <v>20</v>
+      </c>
+      <c r="N45" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="46">
@@ -3172,28 +3311,31 @@
         <v>3.79761525E8</v>
       </c>
       <c r="F46" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G46" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H46" t="s">
-        <v>220</v>
-      </c>
-      <c r="I46" t="s">
         <v>221</v>
       </c>
+      <c r="I46" t="n">
+        <v>4.4511934E7</v>
+      </c>
       <c r="J46" t="s">
-        <v>17</v>
+        <v>222</v>
       </c>
       <c r="K46" t="s">
-        <v>222</v>
+        <v>18</v>
       </c>
       <c r="L46" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="M46" t="s">
-        <v>223</v>
+        <v>20</v>
+      </c>
+      <c r="N46" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="47">
@@ -3213,19 +3355,19 @@
         <v>3.84441809E8</v>
       </c>
       <c r="F47" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G47" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H47" t="s">
-        <v>225</v>
-      </c>
-      <c r="I47" t="s">
         <v>226</v>
       </c>
+      <c r="I47" t="n">
+        <v>4.7230818E7</v>
+      </c>
       <c r="J47" t="s">
-        <v>17</v>
+        <v>227</v>
       </c>
       <c r="K47" t="s">
         <v>18</v>
@@ -3234,7 +3376,10 @@
         <v>19</v>
       </c>
       <c r="M47" t="s">
-        <v>227</v>
+        <v>20</v>
+      </c>
+      <c r="N47" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="48">
@@ -3254,19 +3399,19 @@
         <v>4.07669688E8</v>
       </c>
       <c r="F48" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G48" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H48" t="s">
-        <v>230</v>
-      </c>
-      <c r="I48" t="s">
         <v>231</v>
       </c>
+      <c r="I48" t="n">
+        <v>4.8582356E7</v>
+      </c>
       <c r="J48" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
       <c r="K48" t="s">
         <v>18</v>
@@ -3275,7 +3420,10 @@
         <v>19</v>
       </c>
       <c r="M48" t="s">
-        <v>140</v>
+        <v>20</v>
+      </c>
+      <c r="N48" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="49">
@@ -3295,28 +3443,31 @@
         <v>4.1515437E8</v>
       </c>
       <c r="F49" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G49" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H49" t="s">
-        <v>220</v>
-      </c>
-      <c r="I49" t="s">
         <v>221</v>
       </c>
+      <c r="I49" t="n">
+        <v>4.4511934E7</v>
+      </c>
       <c r="J49" t="s">
-        <v>17</v>
+        <v>222</v>
       </c>
       <c r="K49" t="s">
-        <v>222</v>
+        <v>18</v>
       </c>
       <c r="L49" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="M49" t="s">
-        <v>223</v>
+        <v>20</v>
+      </c>
+      <c r="N49" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="50">
@@ -3336,19 +3487,19 @@
         <v>4.16564537E8</v>
       </c>
       <c r="F50" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H50" t="s">
-        <v>234</v>
-      </c>
-      <c r="I50" t="s">
         <v>235</v>
       </c>
+      <c r="I50" t="n">
+        <v>5.0354754E7</v>
+      </c>
       <c r="J50" t="s">
-        <v>17</v>
+        <v>236</v>
       </c>
       <c r="K50" t="s">
         <v>18</v>
@@ -3357,7 +3508,10 @@
         <v>19</v>
       </c>
       <c r="M50" t="s">
-        <v>236</v>
+        <v>20</v>
+      </c>
+      <c r="N50" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="51">
@@ -3377,19 +3531,19 @@
         <v>4.16989412E8</v>
       </c>
       <c r="F51" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G51" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H51" t="s">
-        <v>239</v>
-      </c>
-      <c r="I51" t="s">
         <v>240</v>
       </c>
+      <c r="I51" t="n">
+        <v>5.0447515E7</v>
+      </c>
       <c r="J51" t="s">
-        <v>17</v>
+        <v>241</v>
       </c>
       <c r="K51" t="s">
         <v>18</v>
@@ -3398,7 +3552,10 @@
         <v>19</v>
       </c>
       <c r="M51" t="s">
-        <v>126</v>
+        <v>20</v>
+      </c>
+      <c r="N51" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="52">
@@ -3418,19 +3575,19 @@
         <v>3.41758296E8</v>
       </c>
       <c r="F52" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G52" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H52" t="s">
-        <v>243</v>
-      </c>
-      <c r="I52" t="s">
         <v>244</v>
       </c>
+      <c r="I52" t="n">
+        <v>4.5448221E7</v>
+      </c>
       <c r="J52" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="K52" t="s">
         <v>18</v>
@@ -3439,7 +3596,10 @@
         <v>19</v>
       </c>
       <c r="M52" t="s">
-        <v>245</v>
+        <v>20</v>
+      </c>
+      <c r="N52" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="53">
@@ -3459,19 +3619,19 @@
         <v>3.65836212E8</v>
       </c>
       <c r="F53" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G53" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H53" t="s">
-        <v>247</v>
-      </c>
-      <c r="I53" t="s">
         <v>248</v>
       </c>
+      <c r="I53" t="n">
+        <v>4.6338453E7</v>
+      </c>
       <c r="J53" t="s">
-        <v>17</v>
+        <v>249</v>
       </c>
       <c r="K53" t="s">
         <v>18</v>
@@ -3480,7 +3640,10 @@
         <v>19</v>
       </c>
       <c r="M53" t="s">
-        <v>249</v>
+        <v>20</v>
+      </c>
+      <c r="N53" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="54">
@@ -3500,19 +3663,19 @@
         <v>4.14727847E8</v>
       </c>
       <c r="F54" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G54" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H54" t="s">
-        <v>252</v>
-      </c>
-      <c r="I54" t="s">
         <v>253</v>
       </c>
+      <c r="I54" t="n">
+        <v>5.0011E7</v>
+      </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>254</v>
       </c>
       <c r="K54" t="s">
         <v>18</v>
@@ -3521,7 +3684,10 @@
         <v>19</v>
       </c>
       <c r="M54" t="s">
-        <v>254</v>
+        <v>20</v>
+      </c>
+      <c r="N54" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="55">
@@ -3541,19 +3707,19 @@
         <v>3.36658357E8</v>
       </c>
       <c r="F55" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G55" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H55" t="s">
-        <v>257</v>
-      </c>
-      <c r="I55" t="s">
         <v>258</v>
       </c>
+      <c r="I55" t="n">
+        <v>4.4215146E7</v>
+      </c>
       <c r="J55" t="s">
-        <v>17</v>
+        <v>259</v>
       </c>
       <c r="K55" t="s">
         <v>18</v>
@@ -3562,7 +3728,10 @@
         <v>19</v>
       </c>
       <c r="M55" t="s">
-        <v>259</v>
+        <v>20</v>
+      </c>
+      <c r="N55" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="56">
@@ -3582,19 +3751,19 @@
         <v>4.12306752E8</v>
       </c>
       <c r="F56" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G56" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H56" t="s">
-        <v>262</v>
-      </c>
-      <c r="I56" t="s">
         <v>263</v>
       </c>
+      <c r="I56" t="n">
+        <v>4.9532922E7</v>
+      </c>
       <c r="J56" t="s">
-        <v>17</v>
+        <v>264</v>
       </c>
       <c r="K56" t="s">
         <v>18</v>
@@ -3603,7 +3772,10 @@
         <v>19</v>
       </c>
       <c r="M56" t="s">
-        <v>264</v>
+        <v>20</v>
+      </c>
+      <c r="N56" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="57">
@@ -3623,19 +3795,19 @@
         <v>3.7574279E8</v>
       </c>
       <c r="F57" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G57" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H57" t="s">
-        <v>267</v>
-      </c>
-      <c r="I57" t="s">
         <v>268</v>
       </c>
+      <c r="I57" t="n">
+        <v>4.6510933E7</v>
+      </c>
       <c r="J57" t="s">
-        <v>17</v>
+        <v>269</v>
       </c>
       <c r="K57" t="s">
         <v>18</v>
@@ -3644,7 +3816,10 @@
         <v>19</v>
       </c>
       <c r="M57" t="s">
-        <v>269</v>
+        <v>20</v>
+      </c>
+      <c r="N57" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="58">
@@ -3664,19 +3839,19 @@
         <v>4.05608703E8</v>
       </c>
       <c r="F58" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G58" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H58" t="s">
-        <v>272</v>
-      </c>
-      <c r="I58" t="s">
         <v>273</v>
       </c>
+      <c r="I58" t="n">
+        <v>4.7665476E7</v>
+      </c>
       <c r="J58" t="s">
-        <v>17</v>
+        <v>274</v>
       </c>
       <c r="K58" t="s">
         <v>18</v>
@@ -3685,7 +3860,10 @@
         <v>19</v>
       </c>
       <c r="M58" t="s">
-        <v>274</v>
+        <v>20</v>
+      </c>
+      <c r="N58" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="59">
@@ -3705,19 +3883,19 @@
         <v>4.25429398E8</v>
       </c>
       <c r="F59" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G59" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H59" t="s">
-        <v>277</v>
-      </c>
-      <c r="I59" t="s">
         <v>278</v>
       </c>
+      <c r="I59" t="n">
+        <v>5.2254308E7</v>
+      </c>
       <c r="J59" t="s">
-        <v>17</v>
+        <v>279</v>
       </c>
       <c r="K59" t="s">
         <v>18</v>
@@ -3726,7 +3904,10 @@
         <v>19</v>
       </c>
       <c r="M59" t="s">
-        <v>279</v>
+        <v>20</v>
+      </c>
+      <c r="N59" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="60">
@@ -3746,19 +3927,19 @@
         <v>3.36768E8</v>
       </c>
       <c r="F60" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G60" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H60" t="s">
-        <v>282</v>
-      </c>
-      <c r="I60" t="s">
         <v>283</v>
       </c>
+      <c r="I60" t="n">
+        <v>4.4316677E7</v>
+      </c>
       <c r="J60" t="s">
-        <v>17</v>
+        <v>284</v>
       </c>
       <c r="K60" t="s">
         <v>18</v>
@@ -3767,7 +3948,10 @@
         <v>19</v>
       </c>
       <c r="M60" t="s">
-        <v>284</v>
+        <v>20</v>
+      </c>
+      <c r="N60" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="61">
@@ -3787,19 +3971,19 @@
         <v>4.40864114E8</v>
       </c>
       <c r="F61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G61" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H61" t="s">
-        <v>287</v>
-      </c>
-      <c r="I61" t="s">
         <v>288</v>
       </c>
+      <c r="I61" t="n">
+        <v>5.3239989E7</v>
+      </c>
       <c r="J61" t="s">
-        <v>17</v>
+        <v>289</v>
       </c>
       <c r="K61" t="s">
         <v>18</v>
@@ -3808,7 +3992,10 @@
         <v>19</v>
       </c>
       <c r="M61" t="s">
-        <v>289</v>
+        <v>20</v>
+      </c>
+      <c r="N61" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="62">
@@ -3828,19 +4015,19 @@
         <v>4.13638895E8</v>
       </c>
       <c r="F62" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G62" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H62" t="s">
-        <v>292</v>
-      </c>
-      <c r="I62" t="s">
         <v>293</v>
       </c>
+      <c r="I62" t="n">
+        <v>4.9791015E7</v>
+      </c>
       <c r="J62" t="s">
-        <v>17</v>
+        <v>294</v>
       </c>
       <c r="K62" t="s">
         <v>18</v>
@@ -3849,7 +4036,10 @@
         <v>19</v>
       </c>
       <c r="M62" t="s">
-        <v>294</v>
+        <v>20</v>
+      </c>
+      <c r="N62" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="63">
@@ -3869,19 +4059,19 @@
         <v>4.17468592E8</v>
       </c>
       <c r="F63" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G63" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H63" t="s">
-        <v>297</v>
-      </c>
-      <c r="I63" t="s">
         <v>298</v>
       </c>
+      <c r="I63" t="n">
+        <v>5.0567904E7</v>
+      </c>
       <c r="J63" t="s">
-        <v>17</v>
+        <v>299</v>
       </c>
       <c r="K63" t="s">
         <v>18</v>
@@ -3890,7 +4080,10 @@
         <v>19</v>
       </c>
       <c r="M63" t="s">
-        <v>299</v>
+        <v>20</v>
+      </c>
+      <c r="N63" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="64">
@@ -3910,19 +4103,19 @@
         <v>4.19048591E8</v>
       </c>
       <c r="F64" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H64" t="s">
-        <v>301</v>
-      </c>
-      <c r="I64" t="s">
         <v>302</v>
       </c>
+      <c r="I64" t="n">
+        <v>5.0906239E7</v>
+      </c>
       <c r="J64" t="s">
-        <v>17</v>
+        <v>303</v>
       </c>
       <c r="K64" t="s">
         <v>18</v>
@@ -3931,7 +4124,10 @@
         <v>19</v>
       </c>
       <c r="M64" t="s">
-        <v>51</v>
+        <v>20</v>
+      </c>
+      <c r="N64" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="65">
@@ -3951,19 +4147,19 @@
         <v>4.19048591E8</v>
       </c>
       <c r="F65" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G65" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H65" t="s">
-        <v>301</v>
-      </c>
-      <c r="I65" t="s">
         <v>302</v>
       </c>
+      <c r="I65" t="n">
+        <v>5.0906239E7</v>
+      </c>
       <c r="J65" t="s">
-        <v>17</v>
+        <v>303</v>
       </c>
       <c r="K65" t="s">
         <v>18</v>
@@ -3972,7 +4168,10 @@
         <v>19</v>
       </c>
       <c r="M65" t="s">
-        <v>51</v>
+        <v>20</v>
+      </c>
+      <c r="N65" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="66">
@@ -3992,19 +4191,19 @@
         <v>4.05784597E8</v>
       </c>
       <c r="F66" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G66" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H66" t="s">
-        <v>305</v>
-      </c>
-      <c r="I66" t="s">
         <v>306</v>
       </c>
+      <c r="I66" t="n">
+        <v>4.8021922E7</v>
+      </c>
       <c r="J66" t="s">
-        <v>17</v>
+        <v>307</v>
       </c>
       <c r="K66" t="s">
         <v>18</v>
@@ -4013,7 +4212,10 @@
         <v>19</v>
       </c>
       <c r="M66" t="s">
-        <v>86</v>
+        <v>20</v>
+      </c>
+      <c r="N66" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="67">
@@ -4033,19 +4235,19 @@
         <v>4.16368441E8</v>
       </c>
       <c r="F67" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G67" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H67" t="s">
-        <v>308</v>
-      </c>
-      <c r="I67" t="s">
         <v>309</v>
       </c>
+      <c r="I67" t="n">
+        <v>5.0321152E7</v>
+      </c>
       <c r="J67" t="s">
-        <v>17</v>
+        <v>310</v>
       </c>
       <c r="K67" t="s">
         <v>18</v>
@@ -4054,7 +4256,10 @@
         <v>19</v>
       </c>
       <c r="M67" t="s">
-        <v>310</v>
+        <v>20</v>
+      </c>
+      <c r="N67" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="68">
@@ -4074,19 +4279,19 @@
         <v>4.16815513E8</v>
       </c>
       <c r="F68" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G68" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H68" t="s">
-        <v>313</v>
-      </c>
-      <c r="I68" t="s">
         <v>314</v>
       </c>
+      <c r="I68" t="n">
+        <v>5.040743E7</v>
+      </c>
       <c r="J68" t="s">
-        <v>17</v>
+        <v>315</v>
       </c>
       <c r="K68" t="s">
         <v>18</v>
@@ -4095,7 +4300,10 @@
         <v>19</v>
       </c>
       <c r="M68" t="s">
-        <v>315</v>
+        <v>20</v>
+      </c>
+      <c r="N68" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="69">
@@ -4115,28 +4323,31 @@
         <v>2.77258962E8</v>
       </c>
       <c r="F69" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H69" t="s">
-        <v>318</v>
-      </c>
-      <c r="I69" t="s">
         <v>319</v>
+      </c>
+      <c r="I69" t="n">
+        <v>3.99335E7</v>
       </c>
       <c r="J69" t="s">
         <v>320</v>
       </c>
       <c r="K69" t="s">
-        <v>18</v>
+        <v>321</v>
       </c>
       <c r="L69" t="s">
-        <v>321</v>
+        <v>19</v>
       </c>
       <c r="M69" t="s">
         <v>322</v>
+      </c>
+      <c r="N69" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="70">
@@ -4156,19 +4367,19 @@
         <v>3.33967698E8</v>
       </c>
       <c r="F70" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G70" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H70" t="s">
-        <v>325</v>
-      </c>
-      <c r="I70" t="s">
         <v>326</v>
       </c>
+      <c r="I70" t="n">
+        <v>4.3710684E7</v>
+      </c>
       <c r="J70" t="s">
-        <v>17</v>
+        <v>327</v>
       </c>
       <c r="K70" t="s">
         <v>18</v>
@@ -4177,7 +4388,10 @@
         <v>19</v>
       </c>
       <c r="M70" t="s">
-        <v>327</v>
+        <v>20</v>
+      </c>
+      <c r="N70" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="71">
@@ -4197,19 +4411,19 @@
         <v>4.05598338E8</v>
       </c>
       <c r="F71" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G71" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H71" t="s">
-        <v>329</v>
-      </c>
-      <c r="I71" t="s">
         <v>330</v>
       </c>
+      <c r="I71" t="n">
+        <v>4.7765939E7</v>
+      </c>
       <c r="J71" t="s">
-        <v>17</v>
+        <v>331</v>
       </c>
       <c r="K71" t="s">
         <v>18</v>
@@ -4218,7 +4432,10 @@
         <v>19</v>
       </c>
       <c r="M71" t="s">
-        <v>331</v>
+        <v>20</v>
+      </c>
+      <c r="N71" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="72">
@@ -4238,19 +4455,19 @@
         <v>3.52680521E8</v>
       </c>
       <c r="F72" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G72" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H72" t="s">
-        <v>334</v>
-      </c>
-      <c r="I72" t="s">
         <v>335</v>
       </c>
+      <c r="I72" t="n">
+        <v>4.5760883E7</v>
+      </c>
       <c r="J72" t="s">
-        <v>17</v>
+        <v>336</v>
       </c>
       <c r="K72" t="s">
         <v>18</v>
@@ -4259,7 +4476,10 @@
         <v>19</v>
       </c>
       <c r="M72" t="s">
-        <v>336</v>
+        <v>20</v>
+      </c>
+      <c r="N72" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="73">
@@ -4279,19 +4499,19 @@
         <v>3.84434927E8</v>
       </c>
       <c r="F73" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G73" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H73" t="s">
-        <v>338</v>
-      </c>
-      <c r="I73" t="s">
         <v>339</v>
       </c>
+      <c r="I73" t="n">
+        <v>4.7199117E7</v>
+      </c>
       <c r="J73" t="s">
-        <v>17</v>
+        <v>340</v>
       </c>
       <c r="K73" t="s">
         <v>18</v>
@@ -4300,7 +4520,10 @@
         <v>19</v>
       </c>
       <c r="M73" t="s">
-        <v>340</v>
+        <v>20</v>
+      </c>
+      <c r="N73" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="74">
@@ -4320,19 +4543,19 @@
         <v>4.07665131E8</v>
       </c>
       <c r="F74" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G74" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H74" t="s">
-        <v>342</v>
-      </c>
-      <c r="I74" t="s">
         <v>343</v>
       </c>
+      <c r="I74" t="n">
+        <v>4.8587819E7</v>
+      </c>
       <c r="J74" t="s">
-        <v>17</v>
+        <v>344</v>
       </c>
       <c r="K74" t="s">
         <v>18</v>
@@ -4341,7 +4564,10 @@
         <v>19</v>
       </c>
       <c r="M74" t="s">
-        <v>344</v>
+        <v>20</v>
+      </c>
+      <c r="N74" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="75">
@@ -4361,28 +4587,31 @@
         <v>4.22599862E8</v>
       </c>
       <c r="F75" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G75" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H75" t="s">
-        <v>347</v>
-      </c>
-      <c r="I75" t="s">
         <v>348</v>
       </c>
+      <c r="I75" t="n">
+        <v>5.1657388E7</v>
+      </c>
       <c r="J75" t="s">
-        <v>320</v>
+        <v>349</v>
       </c>
       <c r="K75" t="s">
-        <v>18</v>
+        <v>321</v>
       </c>
       <c r="L75" t="s">
-        <v>321</v>
+        <v>19</v>
       </c>
       <c r="M75" t="s">
-        <v>349</v>
+        <v>322</v>
+      </c>
+      <c r="N75" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="76">
@@ -4402,19 +4631,19 @@
         <v>3.81151747E8</v>
       </c>
       <c r="F76" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G76" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="H76" t="s">
-        <v>352</v>
-      </c>
-      <c r="I76" t="s">
         <v>353</v>
       </c>
+      <c r="I76" t="n">
+        <v>4.6773129E7</v>
+      </c>
       <c r="J76" t="s">
-        <v>17</v>
+        <v>354</v>
       </c>
       <c r="K76" t="s">
         <v>18</v>
@@ -4423,7 +4652,10 @@
         <v>19</v>
       </c>
       <c r="M76" t="s">
-        <v>354</v>
+        <v>20</v>
+      </c>
+      <c r="N76" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="77">
@@ -4443,19 +4675,19 @@
         <v>3.8162995E8</v>
       </c>
       <c r="F77" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="G77" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H77" t="s">
-        <v>357</v>
-      </c>
-      <c r="I77" t="s">
         <v>358</v>
       </c>
+      <c r="I77" t="n">
+        <v>4.7124207E7</v>
+      </c>
       <c r="J77" t="s">
-        <v>17</v>
+        <v>359</v>
       </c>
       <c r="K77" t="s">
         <v>18</v>
@@ -4464,7 +4696,10 @@
         <v>19</v>
       </c>
       <c r="M77" t="s">
-        <v>359</v>
+        <v>20</v>
+      </c>
+      <c r="N77" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="78">
@@ -4484,19 +4719,19 @@
         <v>4.0711782E8</v>
       </c>
       <c r="F78" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G78" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H78" t="s">
-        <v>362</v>
-      </c>
-      <c r="I78" t="s">
         <v>363</v>
       </c>
+      <c r="I78" t="n">
+        <v>4.8454678E7</v>
+      </c>
       <c r="J78" t="s">
-        <v>17</v>
+        <v>364</v>
       </c>
       <c r="K78" t="s">
         <v>18</v>
@@ -4505,7 +4740,10 @@
         <v>19</v>
       </c>
       <c r="M78" t="s">
-        <v>364</v>
+        <v>20</v>
+      </c>
+      <c r="N78" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="79">
@@ -4525,19 +4763,19 @@
         <v>3.41975587E8</v>
       </c>
       <c r="F79" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G79" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H79" t="s">
-        <v>367</v>
-      </c>
-      <c r="I79" t="s">
         <v>368</v>
       </c>
+      <c r="I79" t="n">
+        <v>4.5483905E7</v>
+      </c>
       <c r="J79" t="s">
-        <v>17</v>
+        <v>369</v>
       </c>
       <c r="K79" t="s">
         <v>18</v>
@@ -4546,7 +4784,10 @@
         <v>19</v>
       </c>
       <c r="M79" t="s">
-        <v>369</v>
+        <v>20</v>
+      </c>
+      <c r="N79" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="80">
@@ -4566,19 +4807,19 @@
         <v>3.65413218E8</v>
       </c>
       <c r="F80" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G80" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H80" t="s">
-        <v>371</v>
-      </c>
-      <c r="I80" t="s">
         <v>372</v>
       </c>
+      <c r="I80" t="n">
+        <v>4.6152832E7</v>
+      </c>
       <c r="J80" t="s">
-        <v>17</v>
+        <v>373</v>
       </c>
       <c r="K80" t="s">
         <v>18</v>
@@ -4587,7 +4828,10 @@
         <v>19</v>
       </c>
       <c r="M80" t="s">
-        <v>373</v>
+        <v>20</v>
+      </c>
+      <c r="N80" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="81">
@@ -4607,19 +4851,19 @@
         <v>3.65923468E8</v>
       </c>
       <c r="F81" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G81" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H81" t="s">
-        <v>375</v>
-      </c>
-      <c r="I81" t="s">
         <v>376</v>
       </c>
+      <c r="I81" t="n">
+        <v>4.6349264E7</v>
+      </c>
       <c r="J81" t="s">
-        <v>17</v>
+        <v>377</v>
       </c>
       <c r="K81" t="s">
         <v>18</v>
@@ -4628,7 +4872,10 @@
         <v>19</v>
       </c>
       <c r="M81" t="s">
-        <v>377</v>
+        <v>20</v>
+      </c>
+      <c r="N81" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="82">
@@ -4648,28 +4895,31 @@
         <v>4.08982321E8</v>
       </c>
       <c r="F82" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G82" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H82" t="s">
-        <v>380</v>
-      </c>
-      <c r="I82" t="s">
         <v>381</v>
       </c>
+      <c r="I82" t="n">
+        <v>4.6349331E7</v>
+      </c>
       <c r="J82" t="s">
-        <v>320</v>
+        <v>382</v>
       </c>
       <c r="K82" t="s">
-        <v>18</v>
+        <v>321</v>
       </c>
       <c r="L82" t="s">
-        <v>321</v>
+        <v>19</v>
       </c>
       <c r="M82" t="s">
-        <v>274</v>
+        <v>322</v>
+      </c>
+      <c r="N82" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="83">
@@ -4689,19 +4939,19 @@
         <v>3.34788937E8</v>
       </c>
       <c r="F83" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G83" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H83" t="s">
-        <v>384</v>
-      </c>
-      <c r="I83" t="s">
         <v>385</v>
       </c>
+      <c r="I83" t="n">
+        <v>4.3911135E7</v>
+      </c>
       <c r="J83" t="s">
-        <v>17</v>
+        <v>386</v>
       </c>
       <c r="K83" t="s">
         <v>18</v>
@@ -4710,7 +4960,10 @@
         <v>19</v>
       </c>
       <c r="M83" t="s">
-        <v>259</v>
+        <v>20</v>
+      </c>
+      <c r="N83" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="84">
@@ -4730,19 +4983,19 @@
         <v>3.65767908E8</v>
       </c>
       <c r="F84" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G84" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H84" t="s">
-        <v>387</v>
-      </c>
-      <c r="I84" t="s">
         <v>388</v>
       </c>
+      <c r="I84" t="n">
+        <v>4.6292683E7</v>
+      </c>
       <c r="J84" t="s">
-        <v>17</v>
+        <v>389</v>
       </c>
       <c r="K84" t="s">
         <v>18</v>
@@ -4751,7 +5004,10 @@
         <v>19</v>
       </c>
       <c r="M84" t="s">
-        <v>344</v>
+        <v>20</v>
+      </c>
+      <c r="N84" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="85">
@@ -4771,19 +5027,19 @@
         <v>4.05598338E8</v>
       </c>
       <c r="F85" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G85" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H85" t="s">
-        <v>329</v>
-      </c>
-      <c r="I85" t="s">
         <v>330</v>
       </c>
+      <c r="I85" t="n">
+        <v>4.7765939E7</v>
+      </c>
       <c r="J85" t="s">
-        <v>17</v>
+        <v>331</v>
       </c>
       <c r="K85" t="s">
         <v>18</v>
@@ -4792,7 +5048,10 @@
         <v>19</v>
       </c>
       <c r="M85" t="s">
-        <v>331</v>
+        <v>20</v>
+      </c>
+      <c r="N85" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="86">
@@ -4812,19 +5071,19 @@
         <v>4.06241522E8</v>
       </c>
       <c r="F86" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G86" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H86" t="s">
-        <v>390</v>
-      </c>
-      <c r="I86" t="s">
         <v>391</v>
       </c>
+      <c r="I86" t="n">
+        <v>4.8155313E7</v>
+      </c>
       <c r="J86" t="s">
-        <v>17</v>
+        <v>392</v>
       </c>
       <c r="K86" t="s">
         <v>18</v>
@@ -4833,7 +5092,10 @@
         <v>19</v>
       </c>
       <c r="M86" t="s">
-        <v>392</v>
+        <v>20</v>
+      </c>
+      <c r="N86" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="87">
@@ -4853,19 +5115,19 @@
         <v>4.16358849E8</v>
       </c>
       <c r="F87" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G87" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H87" t="s">
-        <v>394</v>
-      </c>
-      <c r="I87" t="s">
         <v>395</v>
       </c>
+      <c r="I87" t="n">
+        <v>5.0317379E7</v>
+      </c>
       <c r="J87" t="s">
-        <v>17</v>
+        <v>396</v>
       </c>
       <c r="K87" t="s">
         <v>18</v>
@@ -4874,7 +5136,10 @@
         <v>19</v>
       </c>
       <c r="M87" t="s">
-        <v>396</v>
+        <v>20</v>
+      </c>
+      <c r="N87" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="88">
@@ -4894,19 +5159,19 @@
         <v>3.65786643E8</v>
       </c>
       <c r="F88" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G88" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H88" t="s">
-        <v>398</v>
-      </c>
-      <c r="I88" t="s">
         <v>399</v>
       </c>
+      <c r="I88" t="n">
+        <v>4.6349451E7</v>
+      </c>
       <c r="J88" t="s">
-        <v>17</v>
+        <v>400</v>
       </c>
       <c r="K88" t="s">
         <v>18</v>
@@ -4915,7 +5180,10 @@
         <v>19</v>
       </c>
       <c r="M88" t="s">
-        <v>400</v>
+        <v>20</v>
+      </c>
+      <c r="N88" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="89">
@@ -4935,19 +5203,19 @@
         <v>4.20823414E8</v>
       </c>
       <c r="F89" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G89" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H89" t="s">
-        <v>403</v>
-      </c>
-      <c r="I89" t="s">
         <v>404</v>
       </c>
+      <c r="I89" t="n">
+        <v>5.127716E7</v>
+      </c>
       <c r="J89" t="s">
-        <v>17</v>
+        <v>405</v>
       </c>
       <c r="K89" t="s">
         <v>18</v>
@@ -4956,7 +5224,10 @@
         <v>19</v>
       </c>
       <c r="M89" t="s">
-        <v>405</v>
+        <v>20</v>
+      </c>
+      <c r="N89" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="90">
@@ -4976,28 +5247,31 @@
         <v>4.40603601E8</v>
       </c>
       <c r="F90" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G90" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H90" t="s">
-        <v>408</v>
-      </c>
-      <c r="I90" t="s">
         <v>409</v>
       </c>
+      <c r="I90" t="n">
+        <v>5.3124878E7</v>
+      </c>
       <c r="J90" t="s">
-        <v>320</v>
+        <v>410</v>
       </c>
       <c r="K90" t="s">
-        <v>18</v>
+        <v>321</v>
       </c>
       <c r="L90" t="s">
-        <v>321</v>
+        <v>19</v>
       </c>
       <c r="M90" t="s">
-        <v>410</v>
+        <v>322</v>
+      </c>
+      <c r="N90" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new features and outputs
</commit_message>
<xml_diff>
--- a/citations.xlsx
+++ b/citations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="497">
   <si>
     <t>RAP - Citation ID</t>
   </si>
@@ -1269,6 +1269,240 @@
   </si>
   <si>
     <t>2013-11-19</t>
+  </si>
+  <si>
+    <t>102236930</t>
+  </si>
+  <si>
+    <t>2011-11-09</t>
+  </si>
+  <si>
+    <t>201010156707</t>
+  </si>
+  <si>
+    <t>CN20101156707</t>
+  </si>
+  <si>
+    <t>2010-04-27</t>
+  </si>
+  <si>
+    <t>102236931</t>
+  </si>
+  <si>
+    <t>201010156708</t>
+  </si>
+  <si>
+    <t>CN20101156708</t>
+  </si>
+  <si>
+    <t>102236929</t>
+  </si>
+  <si>
+    <t>201010156703</t>
+  </si>
+  <si>
+    <t>CN20101156703</t>
+  </si>
+  <si>
+    <t>102236927</t>
+  </si>
+  <si>
+    <t>201010156697</t>
+  </si>
+  <si>
+    <t>CN20101156697</t>
+  </si>
+  <si>
+    <t>102236928</t>
+  </si>
+  <si>
+    <t>201010156709</t>
+  </si>
+  <si>
+    <t>CN20101156709</t>
+  </si>
+  <si>
+    <t>102254365</t>
+  </si>
+  <si>
+    <t>2011-11-23</t>
+  </si>
+  <si>
+    <t>201010187171</t>
+  </si>
+  <si>
+    <t>CN20101187171</t>
+  </si>
+  <si>
+    <t>2010-05-31</t>
+  </si>
+  <si>
+    <t>102243783</t>
+  </si>
+  <si>
+    <t>2011-11-16</t>
+  </si>
+  <si>
+    <t>201110031148</t>
+  </si>
+  <si>
+    <t>CN2011131148</t>
+  </si>
+  <si>
+    <t>2011-01-28</t>
+  </si>
+  <si>
+    <t>102254139</t>
+  </si>
+  <si>
+    <t>201110029356</t>
+  </si>
+  <si>
+    <t>CN2011129356</t>
+  </si>
+  <si>
+    <t>2011-01-27</t>
+  </si>
+  <si>
+    <t>102254364</t>
+  </si>
+  <si>
+    <t>201010187161</t>
+  </si>
+  <si>
+    <t>CN20101187161</t>
+  </si>
+  <si>
+    <t>102446376</t>
+  </si>
+  <si>
+    <t>2012-05-09</t>
+  </si>
+  <si>
+    <t>201110460383</t>
+  </si>
+  <si>
+    <t>CN20111460383</t>
+  </si>
+  <si>
+    <t>2011-12-31</t>
+  </si>
+  <si>
+    <t>2014048091</t>
+  </si>
+  <si>
+    <t>2014-04-03</t>
+  </si>
+  <si>
+    <t>2013072849</t>
+  </si>
+  <si>
+    <t>WO2013CN72849</t>
+  </si>
+  <si>
+    <t>2013-03-19</t>
+  </si>
+  <si>
+    <t>2012-09-29</t>
+  </si>
+  <si>
+    <t>102542656</t>
+  </si>
+  <si>
+    <t>201110460381</t>
+  </si>
+  <si>
+    <t>CN20111460381</t>
+  </si>
+  <si>
+    <t>102592345</t>
+  </si>
+  <si>
+    <t>2012-07-18</t>
+  </si>
+  <si>
+    <t>201210050503</t>
+  </si>
+  <si>
+    <t>CN2012150503</t>
+  </si>
+  <si>
+    <t>2012-02-29</t>
+  </si>
+  <si>
+    <t>102855705</t>
+  </si>
+  <si>
+    <t>201210344840</t>
+  </si>
+  <si>
+    <t>CN20121344840</t>
+  </si>
+  <si>
+    <t>2012-09-17</t>
+  </si>
+  <si>
+    <t>102855715</t>
+  </si>
+  <si>
+    <t>201210344881</t>
+  </si>
+  <si>
+    <t>CN20121344881</t>
+  </si>
+  <si>
+    <t>102855474</t>
+  </si>
+  <si>
+    <t>201210344770</t>
+  </si>
+  <si>
+    <t>CN20121344770</t>
+  </si>
+  <si>
+    <t>103745523</t>
+  </si>
+  <si>
+    <t>201310733869</t>
+  </si>
+  <si>
+    <t>CN20131733869</t>
+  </si>
+  <si>
+    <t>2013-12-26</t>
+  </si>
+  <si>
+    <t>103745184</t>
+  </si>
+  <si>
+    <t>201310731418</t>
+  </si>
+  <si>
+    <t>CN20131731418</t>
+  </si>
+  <si>
+    <t>103753976</t>
+  </si>
+  <si>
+    <t>2014-04-30</t>
+  </si>
+  <si>
+    <t>201310749712</t>
+  </si>
+  <si>
+    <t>CN20131749712</t>
+  </si>
+  <si>
+    <t>2013-12-31</t>
+  </si>
+  <si>
+    <t>103753975</t>
+  </si>
+  <si>
+    <t>201310737840</t>
+  </si>
+  <si>
+    <t>CN20131737840</t>
   </si>
 </sst>
 </file>
@@ -5566,6 +5800,946 @@
         <v>418</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="B91" t="n">
+        <v>416.0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>3.4020951E8</v>
+      </c>
+      <c r="F91" t="s">
+        <v>419</v>
+      </c>
+      <c r="G91" t="s">
+        <v>420</v>
+      </c>
+      <c r="H91" t="s">
+        <v>421</v>
+      </c>
+      <c r="I91" t="n">
+        <v>4.4887546E7</v>
+      </c>
+      <c r="J91" t="s">
+        <v>422</v>
+      </c>
+      <c r="K91" t="s">
+        <v>19</v>
+      </c>
+      <c r="L91" t="s">
+        <v>20</v>
+      </c>
+      <c r="M91" t="s">
+        <v>21</v>
+      </c>
+      <c r="N91" t="s">
+        <v>423</v>
+      </c>
+      <c r="O91" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="B92" t="n">
+        <v>416.0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>3.40223848E8</v>
+      </c>
+      <c r="F92" t="s">
+        <v>424</v>
+      </c>
+      <c r="G92" t="s">
+        <v>420</v>
+      </c>
+      <c r="H92" t="s">
+        <v>425</v>
+      </c>
+      <c r="I92" t="n">
+        <v>4.4887547E7</v>
+      </c>
+      <c r="J92" t="s">
+        <v>426</v>
+      </c>
+      <c r="K92" t="s">
+        <v>19</v>
+      </c>
+      <c r="L92" t="s">
+        <v>20</v>
+      </c>
+      <c r="M92" t="s">
+        <v>21</v>
+      </c>
+      <c r="N92" t="s">
+        <v>423</v>
+      </c>
+      <c r="O92" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="B93" t="n">
+        <v>416.0</v>
+      </c>
+      <c r="C93" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>3.40223851E8</v>
+      </c>
+      <c r="F93" t="s">
+        <v>427</v>
+      </c>
+      <c r="G93" t="s">
+        <v>420</v>
+      </c>
+      <c r="H93" t="s">
+        <v>428</v>
+      </c>
+      <c r="I93" t="n">
+        <v>4.4887545E7</v>
+      </c>
+      <c r="J93" t="s">
+        <v>429</v>
+      </c>
+      <c r="K93" t="s">
+        <v>19</v>
+      </c>
+      <c r="L93" t="s">
+        <v>20</v>
+      </c>
+      <c r="M93" t="s">
+        <v>21</v>
+      </c>
+      <c r="N93" t="s">
+        <v>423</v>
+      </c>
+      <c r="O93" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="B94" t="n">
+        <v>416.0</v>
+      </c>
+      <c r="C94" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>3.40223853E8</v>
+      </c>
+      <c r="F94" t="s">
+        <v>430</v>
+      </c>
+      <c r="G94" t="s">
+        <v>420</v>
+      </c>
+      <c r="H94" t="s">
+        <v>431</v>
+      </c>
+      <c r="I94" t="n">
+        <v>4.4887543E7</v>
+      </c>
+      <c r="J94" t="s">
+        <v>432</v>
+      </c>
+      <c r="K94" t="s">
+        <v>19</v>
+      </c>
+      <c r="L94" t="s">
+        <v>20</v>
+      </c>
+      <c r="M94" t="s">
+        <v>21</v>
+      </c>
+      <c r="N94" t="s">
+        <v>423</v>
+      </c>
+      <c r="O94" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="B95" t="n">
+        <v>416.0</v>
+      </c>
+      <c r="C95" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>3.40239245E8</v>
+      </c>
+      <c r="F95" t="s">
+        <v>433</v>
+      </c>
+      <c r="G95" t="s">
+        <v>420</v>
+      </c>
+      <c r="H95" t="s">
+        <v>434</v>
+      </c>
+      <c r="I95" t="n">
+        <v>4.4887544E7</v>
+      </c>
+      <c r="J95" t="s">
+        <v>435</v>
+      </c>
+      <c r="K95" t="s">
+        <v>19</v>
+      </c>
+      <c r="L95" t="s">
+        <v>20</v>
+      </c>
+      <c r="M95" t="s">
+        <v>21</v>
+      </c>
+      <c r="N95" t="s">
+        <v>423</v>
+      </c>
+      <c r="O95" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="B96" t="n">
+        <v>418.0</v>
+      </c>
+      <c r="C96" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>3.40587244E8</v>
+      </c>
+      <c r="F96" t="s">
+        <v>436</v>
+      </c>
+      <c r="G96" t="s">
+        <v>437</v>
+      </c>
+      <c r="H96" t="s">
+        <v>438</v>
+      </c>
+      <c r="I96" t="n">
+        <v>4.4981606E7</v>
+      </c>
+      <c r="J96" t="s">
+        <v>439</v>
+      </c>
+      <c r="K96" t="s">
+        <v>19</v>
+      </c>
+      <c r="L96" t="s">
+        <v>20</v>
+      </c>
+      <c r="M96" t="s">
+        <v>21</v>
+      </c>
+      <c r="N96" t="s">
+        <v>440</v>
+      </c>
+      <c r="O96" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="B97" t="n">
+        <v>418.0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E97" t="n">
+        <v>3.40603798E8</v>
+      </c>
+      <c r="F97" t="s">
+        <v>441</v>
+      </c>
+      <c r="G97" t="s">
+        <v>442</v>
+      </c>
+      <c r="H97" t="s">
+        <v>443</v>
+      </c>
+      <c r="I97" t="n">
+        <v>4.496182E7</v>
+      </c>
+      <c r="J97" t="s">
+        <v>444</v>
+      </c>
+      <c r="K97" t="s">
+        <v>19</v>
+      </c>
+      <c r="L97" t="s">
+        <v>20</v>
+      </c>
+      <c r="M97" t="s">
+        <v>21</v>
+      </c>
+      <c r="N97" t="s">
+        <v>445</v>
+      </c>
+      <c r="O97" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="B98" t="n">
+        <v>419.0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E98" t="n">
+        <v>3.40399151E8</v>
+      </c>
+      <c r="F98" t="s">
+        <v>446</v>
+      </c>
+      <c r="G98" t="s">
+        <v>437</v>
+      </c>
+      <c r="H98" t="s">
+        <v>447</v>
+      </c>
+      <c r="I98" t="n">
+        <v>4.4981395E7</v>
+      </c>
+      <c r="J98" t="s">
+        <v>448</v>
+      </c>
+      <c r="K98" t="s">
+        <v>19</v>
+      </c>
+      <c r="L98" t="s">
+        <v>20</v>
+      </c>
+      <c r="M98" t="s">
+        <v>21</v>
+      </c>
+      <c r="N98" t="s">
+        <v>449</v>
+      </c>
+      <c r="O98" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="B99" t="n">
+        <v>419.0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>3.4058708E8</v>
+      </c>
+      <c r="F99" t="s">
+        <v>450</v>
+      </c>
+      <c r="G99" t="s">
+        <v>437</v>
+      </c>
+      <c r="H99" t="s">
+        <v>451</v>
+      </c>
+      <c r="I99" t="n">
+        <v>4.4981605E7</v>
+      </c>
+      <c r="J99" t="s">
+        <v>452</v>
+      </c>
+      <c r="K99" t="s">
+        <v>19</v>
+      </c>
+      <c r="L99" t="s">
+        <v>20</v>
+      </c>
+      <c r="M99" t="s">
+        <v>21</v>
+      </c>
+      <c r="N99" t="s">
+        <v>440</v>
+      </c>
+      <c r="O99" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="B100" t="n">
+        <v>425.0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>3.65088177E8</v>
+      </c>
+      <c r="F100" t="s">
+        <v>453</v>
+      </c>
+      <c r="G100" t="s">
+        <v>454</v>
+      </c>
+      <c r="H100" t="s">
+        <v>455</v>
+      </c>
+      <c r="I100" t="n">
+        <v>4.6008849E7</v>
+      </c>
+      <c r="J100" t="s">
+        <v>456</v>
+      </c>
+      <c r="K100" t="s">
+        <v>19</v>
+      </c>
+      <c r="L100" t="s">
+        <v>20</v>
+      </c>
+      <c r="M100" t="s">
+        <v>21</v>
+      </c>
+      <c r="N100" t="s">
+        <v>457</v>
+      </c>
+      <c r="O100" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="B101" t="n">
+        <v>425.0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D101" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>4.16676405E8</v>
+      </c>
+      <c r="F101" t="s">
+        <v>458</v>
+      </c>
+      <c r="G101" t="s">
+        <v>459</v>
+      </c>
+      <c r="H101" t="s">
+        <v>460</v>
+      </c>
+      <c r="I101" t="n">
+        <v>4.8021925E7</v>
+      </c>
+      <c r="J101" t="s">
+        <v>461</v>
+      </c>
+      <c r="K101" t="s">
+        <v>325</v>
+      </c>
+      <c r="L101" t="s">
+        <v>20</v>
+      </c>
+      <c r="M101" t="s">
+        <v>326</v>
+      </c>
+      <c r="N101" t="s">
+        <v>462</v>
+      </c>
+      <c r="O101" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B102" t="n">
+        <v>426.0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>3.75150168E8</v>
+      </c>
+      <c r="F102" t="s">
+        <v>464</v>
+      </c>
+      <c r="G102" t="s">
+        <v>207</v>
+      </c>
+      <c r="H102" t="s">
+        <v>465</v>
+      </c>
+      <c r="I102" t="n">
+        <v>4.6349462E7</v>
+      </c>
+      <c r="J102" t="s">
+        <v>466</v>
+      </c>
+      <c r="K102" t="s">
+        <v>19</v>
+      </c>
+      <c r="L102" t="s">
+        <v>20</v>
+      </c>
+      <c r="M102" t="s">
+        <v>21</v>
+      </c>
+      <c r="N102" t="s">
+        <v>457</v>
+      </c>
+      <c r="O102" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="B103" t="n">
+        <v>428.0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>3.75747495E8</v>
+      </c>
+      <c r="F103" t="s">
+        <v>467</v>
+      </c>
+      <c r="G103" t="s">
+        <v>468</v>
+      </c>
+      <c r="H103" t="s">
+        <v>469</v>
+      </c>
+      <c r="I103" t="n">
+        <v>4.6480928E7</v>
+      </c>
+      <c r="J103" t="s">
+        <v>470</v>
+      </c>
+      <c r="K103" t="s">
+        <v>19</v>
+      </c>
+      <c r="L103" t="s">
+        <v>20</v>
+      </c>
+      <c r="M103" t="s">
+        <v>21</v>
+      </c>
+      <c r="N103" t="s">
+        <v>471</v>
+      </c>
+      <c r="O103" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="B104" t="n">
+        <v>435.0</v>
+      </c>
+      <c r="C104" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>3.84486619E8</v>
+      </c>
+      <c r="F104" t="s">
+        <v>472</v>
+      </c>
+      <c r="G104" t="s">
+        <v>221</v>
+      </c>
+      <c r="H104" t="s">
+        <v>473</v>
+      </c>
+      <c r="I104" t="n">
+        <v>4.7402258E7</v>
+      </c>
+      <c r="J104" t="s">
+        <v>474</v>
+      </c>
+      <c r="K104" t="s">
+        <v>19</v>
+      </c>
+      <c r="L104" t="s">
+        <v>20</v>
+      </c>
+      <c r="M104" t="s">
+        <v>21</v>
+      </c>
+      <c r="N104" t="s">
+        <v>475</v>
+      </c>
+      <c r="O104" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="B105" t="n">
+        <v>436.0</v>
+      </c>
+      <c r="C105" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D105" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>3.84486622E8</v>
+      </c>
+      <c r="F105" t="s">
+        <v>476</v>
+      </c>
+      <c r="G105" t="s">
+        <v>221</v>
+      </c>
+      <c r="H105" t="s">
+        <v>477</v>
+      </c>
+      <c r="I105" t="n">
+        <v>4.7402263E7</v>
+      </c>
+      <c r="J105" t="s">
+        <v>478</v>
+      </c>
+      <c r="K105" t="s">
+        <v>19</v>
+      </c>
+      <c r="L105" t="s">
+        <v>20</v>
+      </c>
+      <c r="M105" t="s">
+        <v>21</v>
+      </c>
+      <c r="N105" t="s">
+        <v>475</v>
+      </c>
+      <c r="O105" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="B106" t="n">
+        <v>437.0</v>
+      </c>
+      <c r="C106" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D106" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>3.84486513E8</v>
+      </c>
+      <c r="F106" t="s">
+        <v>479</v>
+      </c>
+      <c r="G106" t="s">
+        <v>221</v>
+      </c>
+      <c r="H106" t="s">
+        <v>480</v>
+      </c>
+      <c r="I106" t="n">
+        <v>4.7402052E7</v>
+      </c>
+      <c r="J106" t="s">
+        <v>481</v>
+      </c>
+      <c r="K106" t="s">
+        <v>19</v>
+      </c>
+      <c r="L106" t="s">
+        <v>20</v>
+      </c>
+      <c r="M106" t="s">
+        <v>21</v>
+      </c>
+      <c r="N106" t="s">
+        <v>475</v>
+      </c>
+      <c r="O106" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="B107" t="n">
+        <v>447.0</v>
+      </c>
+      <c r="C107" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>4.17197591E8</v>
+      </c>
+      <c r="F107" t="s">
+        <v>482</v>
+      </c>
+      <c r="G107" t="s">
+        <v>110</v>
+      </c>
+      <c r="H107" t="s">
+        <v>483</v>
+      </c>
+      <c r="I107" t="n">
+        <v>5.0502538E7</v>
+      </c>
+      <c r="J107" t="s">
+        <v>484</v>
+      </c>
+      <c r="K107" t="s">
+        <v>19</v>
+      </c>
+      <c r="L107" t="s">
+        <v>20</v>
+      </c>
+      <c r="M107" t="s">
+        <v>21</v>
+      </c>
+      <c r="N107" t="s">
+        <v>485</v>
+      </c>
+      <c r="O107" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="B108" t="n">
+        <v>450.0</v>
+      </c>
+      <c r="C108" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>4.17196913E8</v>
+      </c>
+      <c r="F108" t="s">
+        <v>486</v>
+      </c>
+      <c r="G108" t="s">
+        <v>110</v>
+      </c>
+      <c r="H108" t="s">
+        <v>487</v>
+      </c>
+      <c r="I108" t="n">
+        <v>5.0502201E7</v>
+      </c>
+      <c r="J108" t="s">
+        <v>488</v>
+      </c>
+      <c r="K108" t="s">
+        <v>19</v>
+      </c>
+      <c r="L108" t="s">
+        <v>20</v>
+      </c>
+      <c r="M108" t="s">
+        <v>21</v>
+      </c>
+      <c r="N108" t="s">
+        <v>485</v>
+      </c>
+      <c r="O108" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="B109" t="n">
+        <v>451.0</v>
+      </c>
+      <c r="C109" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>4.17291724E8</v>
+      </c>
+      <c r="F109" t="s">
+        <v>489</v>
+      </c>
+      <c r="G109" t="s">
+        <v>490</v>
+      </c>
+      <c r="H109" t="s">
+        <v>491</v>
+      </c>
+      <c r="I109" t="n">
+        <v>5.0521363E7</v>
+      </c>
+      <c r="J109" t="s">
+        <v>492</v>
+      </c>
+      <c r="K109" t="s">
+        <v>19</v>
+      </c>
+      <c r="L109" t="s">
+        <v>20</v>
+      </c>
+      <c r="M109" t="s">
+        <v>21</v>
+      </c>
+      <c r="N109" t="s">
+        <v>493</v>
+      </c>
+      <c r="O109" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="B110" t="n">
+        <v>456.0</v>
+      </c>
+      <c r="C110" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>4.17291722E8</v>
+      </c>
+      <c r="F110" t="s">
+        <v>494</v>
+      </c>
+      <c r="G110" t="s">
+        <v>490</v>
+      </c>
+      <c r="H110" t="s">
+        <v>495</v>
+      </c>
+      <c r="I110" t="n">
+        <v>5.0521362E7</v>
+      </c>
+      <c r="J110" t="s">
+        <v>496</v>
+      </c>
+      <c r="K110" t="s">
+        <v>19</v>
+      </c>
+      <c r="L110" t="s">
+        <v>20</v>
+      </c>
+      <c r="M110" t="s">
+        <v>21</v>
+      </c>
+      <c r="N110" t="s">
+        <v>485</v>
+      </c>
+      <c r="O110" t="s">
+        <v>485</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed docdb family id query
</commit_message>
<xml_diff>
--- a/citations.xlsx
+++ b/citations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="334">
   <si>
     <t>RAP - Citation ID</t>
   </si>
@@ -392,45 +392,6 @@
     <t>2014-01-17</t>
   </si>
   <si>
-    <t>103465899</t>
-  </si>
-  <si>
-    <t>2013-12-25</t>
-  </si>
-  <si>
-    <t>201310435150</t>
-  </si>
-  <si>
-    <t>CN20131435150</t>
-  </si>
-  <si>
-    <t>2013-09-23</t>
-  </si>
-  <si>
-    <t>103775265</t>
-  </si>
-  <si>
-    <t>2014-05-07</t>
-  </si>
-  <si>
-    <t>201410040221</t>
-  </si>
-  <si>
-    <t>CN2014140221</t>
-  </si>
-  <si>
-    <t>2014-01-27</t>
-  </si>
-  <si>
-    <t>103867307</t>
-  </si>
-  <si>
-    <t>201410128265</t>
-  </si>
-  <si>
-    <t>CN20141128265</t>
-  </si>
-  <si>
     <t>102425877</t>
   </si>
   <si>
@@ -773,48 +734,6 @@
     <t>CN20131739330</t>
   </si>
   <si>
-    <t>102343828</t>
-  </si>
-  <si>
-    <t>2012-02-08</t>
-  </si>
-  <si>
-    <t>201010245479</t>
-  </si>
-  <si>
-    <t>CN20101245479</t>
-  </si>
-  <si>
-    <t>2010-08-04</t>
-  </si>
-  <si>
-    <t>102431462</t>
-  </si>
-  <si>
-    <t>2012-05-02</t>
-  </si>
-  <si>
-    <t>201110311483</t>
-  </si>
-  <si>
-    <t>CN20111311483</t>
-  </si>
-  <si>
-    <t>2011-10-14</t>
-  </si>
-  <si>
-    <t>103358876</t>
-  </si>
-  <si>
-    <t>201210097409</t>
-  </si>
-  <si>
-    <t>CN2012197409</t>
-  </si>
-  <si>
-    <t>2012-03-31</t>
-  </si>
-  <si>
     <t>104279036</t>
   </si>
   <si>
@@ -954,63 +873,6 @@
   </si>
   <si>
     <t>2010-02-05</t>
-  </si>
-  <si>
-    <t>102137309</t>
-  </si>
-  <si>
-    <t>2011-07-27</t>
-  </si>
-  <si>
-    <t>201010569677</t>
-  </si>
-  <si>
-    <t>CN20101569677</t>
-  </si>
-  <si>
-    <t>2010-11-30</t>
-  </si>
-  <si>
-    <t>102196305</t>
-  </si>
-  <si>
-    <t>2011-09-21</t>
-  </si>
-  <si>
-    <t>201010120978</t>
-  </si>
-  <si>
-    <t>CN20101120978</t>
-  </si>
-  <si>
-    <t>2010-03-10</t>
-  </si>
-  <si>
-    <t>102387121</t>
-  </si>
-  <si>
-    <t>201010269887</t>
-  </si>
-  <si>
-    <t>CN20101269887</t>
-  </si>
-  <si>
-    <t>2010-08-30</t>
-  </si>
-  <si>
-    <t>103024590</t>
-  </si>
-  <si>
-    <t>2013-04-03</t>
-  </si>
-  <si>
-    <t>201210530635</t>
-  </si>
-  <si>
-    <t>CN20121530635</t>
-  </si>
-  <si>
-    <t>2012-12-11</t>
   </si>
   <si>
     <t>101790030</t>
@@ -2305,16 +2167,16 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>138.0</v>
+        <v>139.0</v>
       </c>
       <c r="C24" t="n">
         <v>1.0</v>
       </c>
       <c r="D24" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="E24" t="n">
-        <v>4.13638895E8</v>
+        <v>3.63783676E8</v>
       </c>
       <c r="F24" t="s">
         <v>126</v>
@@ -2326,7 +2188,7 @@
         <v>128</v>
       </c>
       <c r="I24" t="n">
-        <v>4.9791015E7</v>
+        <v>4.5959885E7</v>
       </c>
       <c r="J24" t="s">
         <v>129</v>
@@ -2352,31 +2214,31 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>138.0</v>
+        <v>139.0</v>
       </c>
       <c r="C25" t="n">
         <v>1.0</v>
       </c>
       <c r="D25" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="E25" t="n">
-        <v>4.17468592E8</v>
+        <v>3.63783676E8</v>
       </c>
       <c r="F25" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H25" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I25" t="n">
-        <v>5.0567904E7</v>
+        <v>4.5959885E7</v>
       </c>
       <c r="J25" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="K25" t="s">
         <v>19</v>
@@ -2388,10 +2250,10 @@
         <v>21</v>
       </c>
       <c r="N25" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O25" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26">
@@ -2399,31 +2261,31 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>138.0</v>
+        <v>139.0</v>
       </c>
       <c r="C26" t="n">
         <v>1.0</v>
       </c>
       <c r="D26" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="E26" t="n">
-        <v>4.19048591E8</v>
+        <v>4.06971348E8</v>
       </c>
       <c r="F26" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="H26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I26" t="n">
-        <v>5.0906239E7</v>
+        <v>4.8413815E7</v>
       </c>
       <c r="J26" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K26" t="s">
         <v>19</v>
@@ -2435,10 +2297,10 @@
         <v>21</v>
       </c>
       <c r="N26" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="O26" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27">
@@ -2446,31 +2308,31 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>138.0</v>
+        <v>139.0</v>
       </c>
       <c r="C27" t="n">
         <v>1.0</v>
       </c>
       <c r="D27" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="E27" t="n">
-        <v>4.19048591E8</v>
+        <v>4.16080416E8</v>
       </c>
       <c r="F27" t="s">
         <v>136</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="H27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I27" t="n">
-        <v>5.0906239E7</v>
+        <v>5.0249872E7</v>
       </c>
       <c r="J27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K27" t="s">
         <v>19</v>
@@ -2482,10 +2344,10 @@
         <v>21</v>
       </c>
       <c r="N27" t="s">
-        <v>29</v>
+        <v>140</v>
       </c>
       <c r="O27" t="s">
-        <v>29</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28">
@@ -2502,22 +2364,22 @@
         <v>2.0</v>
       </c>
       <c r="E28" t="n">
-        <v>3.63783676E8</v>
+        <v>4.1656423E8</v>
       </c>
       <c r="F28" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G28" t="s">
-        <v>140</v>
+        <v>29</v>
       </c>
       <c r="H28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I28" t="n">
-        <v>4.5959885E7</v>
+        <v>5.0354613E7</v>
       </c>
       <c r="J28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K28" t="s">
         <v>19</v>
@@ -2529,10 +2391,10 @@
         <v>21</v>
       </c>
       <c r="N28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29">
@@ -2540,31 +2402,31 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>139.0</v>
+        <v>140.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
       </c>
       <c r="D29" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="E29" t="n">
-        <v>3.63783676E8</v>
+        <v>3.74890738E8</v>
       </c>
       <c r="F29" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="G29" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="H29" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="I29" t="n">
-        <v>4.5959885E7</v>
+        <v>4.6338113E7</v>
       </c>
       <c r="J29" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="K29" t="s">
         <v>19</v>
@@ -2576,10 +2438,10 @@
         <v>21</v>
       </c>
       <c r="N29" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="O29" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30">
@@ -2587,31 +2449,31 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>139.0</v>
+        <v>140.0</v>
       </c>
       <c r="C30" t="n">
         <v>1.0</v>
       </c>
       <c r="D30" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E30" t="n">
-        <v>4.06971348E8</v>
+        <v>4.21854295E8</v>
       </c>
       <c r="F30" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G30" t="s">
-        <v>145</v>
+        <v>52</v>
       </c>
       <c r="H30" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="I30" t="n">
-        <v>4.8413815E7</v>
+        <v>5.1498007E7</v>
       </c>
       <c r="J30" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="K30" t="s">
         <v>19</v>
@@ -2623,10 +2485,10 @@
         <v>21</v>
       </c>
       <c r="N30" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="O30" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31">
@@ -2634,31 +2496,31 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>139.0</v>
+        <v>141.0</v>
       </c>
       <c r="C31" t="n">
         <v>1.0</v>
       </c>
       <c r="D31" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="E31" t="n">
-        <v>4.16080416E8</v>
+        <v>3.65835465E8</v>
       </c>
       <c r="F31" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G31" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="H31" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="I31" t="n">
-        <v>5.0249872E7</v>
+        <v>4.6294477E7</v>
       </c>
       <c r="J31" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="K31" t="s">
         <v>19</v>
@@ -2670,10 +2532,10 @@
         <v>21</v>
       </c>
       <c r="N31" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="O31" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32">
@@ -2681,31 +2543,31 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="n">
-        <v>139.0</v>
+        <v>141.0</v>
       </c>
       <c r="C32" t="n">
         <v>1.0</v>
       </c>
       <c r="D32" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="E32" t="n">
-        <v>4.1656423E8</v>
+        <v>4.05601631E8</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="G32" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="H32" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="I32" t="n">
-        <v>5.0354613E7</v>
+        <v>4.7760604E7</v>
       </c>
       <c r="J32" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="K32" t="s">
         <v>19</v>
@@ -2717,10 +2579,10 @@
         <v>21</v>
       </c>
       <c r="N32" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O32" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33">
@@ -2728,31 +2590,31 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="n">
-        <v>140.0</v>
+        <v>144.0</v>
       </c>
       <c r="C33" t="n">
         <v>1.0</v>
       </c>
       <c r="D33" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="E33" t="n">
-        <v>3.74890738E8</v>
+        <v>3.53265278E8</v>
       </c>
       <c r="F33" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="G33" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H33" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="I33" t="n">
-        <v>4.6338113E7</v>
+        <v>4.5860248E7</v>
       </c>
       <c r="J33" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="K33" t="s">
         <v>19</v>
@@ -2764,10 +2626,10 @@
         <v>21</v>
       </c>
       <c r="N33" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="O33" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34">
@@ -2775,31 +2637,31 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="n">
-        <v>140.0</v>
+        <v>144.0</v>
       </c>
       <c r="C34" t="n">
         <v>1.0</v>
       </c>
       <c r="D34" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="E34" t="n">
-        <v>4.21854295E8</v>
+        <v>3.7505585E8</v>
       </c>
       <c r="F34" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="G34" t="s">
-        <v>52</v>
+        <v>155</v>
       </c>
       <c r="H34" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="I34" t="n">
-        <v>5.1498007E7</v>
+        <v>4.6289807E7</v>
       </c>
       <c r="J34" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="K34" t="s">
         <v>19</v>
@@ -2811,10 +2673,10 @@
         <v>21</v>
       </c>
       <c r="N34" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="O34" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35">
@@ -2822,31 +2684,31 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="n">
-        <v>141.0</v>
+        <v>144.0</v>
       </c>
       <c r="C35" t="n">
         <v>1.0</v>
       </c>
       <c r="D35" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E35" t="n">
-        <v>3.65835465E8</v>
+        <v>3.80035266E8</v>
       </c>
       <c r="F35" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="G35" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H35" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="I35" t="n">
-        <v>4.6294477E7</v>
+        <v>4.689359E7</v>
       </c>
       <c r="J35" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="K35" t="s">
         <v>19</v>
@@ -2858,10 +2720,10 @@
         <v>21</v>
       </c>
       <c r="N35" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="O35" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36">
@@ -2869,7 +2731,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="n">
-        <v>141.0</v>
+        <v>144.0</v>
       </c>
       <c r="C36" t="n">
         <v>1.0</v>
@@ -2878,22 +2740,22 @@
         <v>5.0</v>
       </c>
       <c r="E36" t="n">
-        <v>4.05601631E8</v>
+        <v>3.80073846E8</v>
       </c>
       <c r="F36" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G36" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H36" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="I36" t="n">
-        <v>4.7760604E7</v>
+        <v>4.6893592E7</v>
       </c>
       <c r="J36" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="K36" t="s">
         <v>19</v>
@@ -2905,10 +2767,10 @@
         <v>21</v>
       </c>
       <c r="N36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="O36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37">
@@ -2922,25 +2784,25 @@
         <v>1.0</v>
       </c>
       <c r="D37" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="E37" t="n">
-        <v>3.53265278E8</v>
+        <v>3.80075929E8</v>
       </c>
       <c r="F37" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G37" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H37" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I37" t="n">
-        <v>4.5860248E7</v>
+        <v>4.6811254E7</v>
       </c>
       <c r="J37" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="K37" t="s">
         <v>19</v>
@@ -2952,10 +2814,10 @@
         <v>21</v>
       </c>
       <c r="N37" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="O37" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38">
@@ -2969,25 +2831,25 @@
         <v>1.0</v>
       </c>
       <c r="D38" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="E38" t="n">
-        <v>3.7505585E8</v>
+        <v>3.80278975E8</v>
       </c>
       <c r="F38" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" t="s">
         <v>182</v>
       </c>
-      <c r="G38" t="s">
-        <v>168</v>
-      </c>
       <c r="H38" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I38" t="n">
-        <v>4.6289807E7</v>
+        <v>4.6811217E7</v>
       </c>
       <c r="J38" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="K38" t="s">
         <v>19</v>
@@ -2999,10 +2861,10 @@
         <v>21</v>
       </c>
       <c r="N38" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="O38" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39">
@@ -3016,25 +2878,25 @@
         <v>1.0</v>
       </c>
       <c r="D39" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="E39" t="n">
-        <v>3.80035266E8</v>
+        <v>3.84461097E8</v>
       </c>
       <c r="F39" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G39" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H39" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I39" t="n">
-        <v>4.689359E7</v>
+        <v>4.7329551E7</v>
       </c>
       <c r="J39" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="K39" t="s">
         <v>19</v>
@@ -3046,10 +2908,10 @@
         <v>21</v>
       </c>
       <c r="N39" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="O39" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40">
@@ -3063,25 +2925,25 @@
         <v>1.0</v>
       </c>
       <c r="D40" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="E40" t="n">
-        <v>3.80073846E8</v>
+        <v>4.10384013E8</v>
       </c>
       <c r="F40" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G40" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="H40" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="I40" t="n">
-        <v>4.6893592E7</v>
+        <v>4.9132785E7</v>
       </c>
       <c r="J40" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="K40" t="s">
         <v>19</v>
@@ -3093,10 +2955,10 @@
         <v>21</v>
       </c>
       <c r="N40" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="O40" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41">
@@ -3110,25 +2972,25 @@
         <v>1.0</v>
       </c>
       <c r="D41" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="E41" t="n">
-        <v>3.80075929E8</v>
+        <v>4.10384015E8</v>
       </c>
       <c r="F41" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G41" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H41" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="I41" t="n">
-        <v>4.6811254E7</v>
+        <v>4.9132786E7</v>
       </c>
       <c r="J41" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="K41" t="s">
         <v>19</v>
@@ -3140,10 +3002,10 @@
         <v>21</v>
       </c>
       <c r="N41" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="O41" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42">
@@ -3157,25 +3019,25 @@
         <v>1.0</v>
       </c>
       <c r="D42" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="E42" t="n">
-        <v>3.80278975E8</v>
+        <v>4.13163522E8</v>
       </c>
       <c r="F42" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="G42" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="H42" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="I42" t="n">
-        <v>4.6811217E7</v>
+        <v>4.9691875E7</v>
       </c>
       <c r="J42" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="K42" t="s">
         <v>19</v>
@@ -3187,10 +3049,10 @@
         <v>21</v>
       </c>
       <c r="N42" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="O42" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43">
@@ -3204,25 +3066,25 @@
         <v>1.0</v>
       </c>
       <c r="D43" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E43" t="n">
-        <v>3.84461097E8</v>
+        <v>4.18808725E8</v>
       </c>
       <c r="F43" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="G43" t="s">
-        <v>204</v>
+        <v>112</v>
       </c>
       <c r="H43" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="I43" t="n">
-        <v>4.7329551E7</v>
+        <v>5.0859177E7</v>
       </c>
       <c r="J43" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="K43" t="s">
         <v>19</v>
@@ -3234,10 +3096,10 @@
         <v>21</v>
       </c>
       <c r="N43" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
       <c r="O43" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44">
@@ -3245,7 +3107,7 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="n">
-        <v>144.0</v>
+        <v>145.0</v>
       </c>
       <c r="C44" t="n">
         <v>1.0</v>
@@ -3254,22 +3116,22 @@
         <v>2.0</v>
       </c>
       <c r="E44" t="n">
-        <v>4.10384013E8</v>
+        <v>3.5300229E8</v>
       </c>
       <c r="F44" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="G44" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H44" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="I44" t="n">
-        <v>4.9132785E7</v>
+        <v>4.5821257E7</v>
       </c>
       <c r="J44" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="K44" t="s">
         <v>19</v>
@@ -3281,10 +3143,10 @@
         <v>21</v>
       </c>
       <c r="N44" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="O44" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45">
@@ -3292,46 +3154,46 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="n">
-        <v>144.0</v>
+        <v>145.0</v>
       </c>
       <c r="C45" t="n">
         <v>1.0</v>
       </c>
       <c r="D45" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E45" t="n">
-        <v>4.10384015E8</v>
+        <v>3.79761525E8</v>
       </c>
       <c r="F45" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="G45" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="H45" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="I45" t="n">
-        <v>4.9132786E7</v>
+        <v>4.4511934E7</v>
       </c>
       <c r="J45" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="K45" t="s">
         <v>19</v>
       </c>
       <c r="L45" t="s">
-        <v>20</v>
+        <v>221</v>
       </c>
       <c r="M45" t="s">
         <v>21</v>
       </c>
       <c r="N45" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="O45" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46">
@@ -3339,31 +3201,31 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="n">
-        <v>144.0</v>
+        <v>145.0</v>
       </c>
       <c r="C46" t="n">
         <v>1.0</v>
       </c>
       <c r="D46" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="E46" t="n">
-        <v>4.13163522E8</v>
+        <v>3.84441809E8</v>
       </c>
       <c r="F46" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G46" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="H46" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="I46" t="n">
-        <v>4.9691875E7</v>
+        <v>4.7230818E7</v>
       </c>
       <c r="J46" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="K46" t="s">
         <v>19</v>
@@ -3375,10 +3237,10 @@
         <v>21</v>
       </c>
       <c r="N46" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="O46" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47">
@@ -3386,31 +3248,31 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="n">
-        <v>144.0</v>
+        <v>145.0</v>
       </c>
       <c r="C47" t="n">
         <v>1.0</v>
       </c>
       <c r="D47" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E47" t="n">
-        <v>4.18808725E8</v>
+        <v>4.07669688E8</v>
       </c>
       <c r="F47" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="G47" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H47" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="I47" t="n">
-        <v>5.0859177E7</v>
+        <v>4.8582356E7</v>
       </c>
       <c r="J47" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K47" t="s">
         <v>19</v>
@@ -3422,10 +3284,10 @@
         <v>21</v>
       </c>
       <c r="N47" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="O47" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48">
@@ -3439,40 +3301,40 @@
         <v>1.0</v>
       </c>
       <c r="D48" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E48" t="n">
-        <v>3.5300229E8</v>
+        <v>4.1515437E8</v>
       </c>
       <c r="F48" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="G48" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="H48" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="I48" t="n">
-        <v>4.5821257E7</v>
+        <v>4.4511934E7</v>
       </c>
       <c r="J48" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="K48" t="s">
         <v>19</v>
       </c>
       <c r="L48" t="s">
-        <v>20</v>
+        <v>221</v>
       </c>
       <c r="M48" t="s">
         <v>21</v>
       </c>
       <c r="N48" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="O48" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49">
@@ -3486,31 +3348,31 @@
         <v>1.0</v>
       </c>
       <c r="D49" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E49" t="n">
-        <v>3.79761525E8</v>
+        <v>4.16564537E8</v>
       </c>
       <c r="F49" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G49" t="s">
-        <v>231</v>
+        <v>29</v>
       </c>
       <c r="H49" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I49" t="n">
-        <v>4.4511934E7</v>
+        <v>5.0354754E7</v>
       </c>
       <c r="J49" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K49" t="s">
         <v>19</v>
       </c>
       <c r="L49" t="s">
-        <v>234</v>
+        <v>20</v>
       </c>
       <c r="M49" t="s">
         <v>21</v>
@@ -3533,25 +3395,25 @@
         <v>1.0</v>
       </c>
       <c r="D50" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E50" t="n">
-        <v>3.84441809E8</v>
+        <v>4.16989412E8</v>
       </c>
       <c r="F50" t="s">
         <v>236</v>
       </c>
       <c r="G50" t="s">
-        <v>107</v>
+        <v>237</v>
       </c>
       <c r="H50" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I50" t="n">
-        <v>4.7230818E7</v>
+        <v>5.0447515E7</v>
       </c>
       <c r="J50" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K50" t="s">
         <v>19</v>
@@ -3563,10 +3425,10 @@
         <v>21</v>
       </c>
       <c r="N50" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
       <c r="O50" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51">
@@ -3574,7 +3436,7 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="n">
-        <v>145.0</v>
+        <v>147.0</v>
       </c>
       <c r="C51" t="n">
         <v>1.0</v>
@@ -3583,7 +3445,7 @@
         <v>3.0</v>
       </c>
       <c r="E51" t="n">
-        <v>4.07669688E8</v>
+        <v>4.25429398E8</v>
       </c>
       <c r="F51" t="s">
         <v>240</v>
@@ -3595,7 +3457,7 @@
         <v>242</v>
       </c>
       <c r="I51" t="n">
-        <v>4.8582356E7</v>
+        <v>5.2254308E7</v>
       </c>
       <c r="J51" t="s">
         <v>243</v>
@@ -3610,10 +3472,10 @@
         <v>21</v>
       </c>
       <c r="N51" t="s">
-        <v>185</v>
+        <v>244</v>
       </c>
       <c r="O51" t="s">
-        <v>185</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52">
@@ -3621,46 +3483,46 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="n">
-        <v>145.0</v>
+        <v>148.0</v>
       </c>
       <c r="C52" t="n">
         <v>1.0</v>
       </c>
       <c r="D52" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="E52" t="n">
-        <v>4.1515437E8</v>
+        <v>3.36658357E8</v>
       </c>
       <c r="F52" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="G52" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H52" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="I52" t="n">
-        <v>4.4511934E7</v>
+        <v>4.4215146E7</v>
       </c>
       <c r="J52" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="K52" t="s">
         <v>19</v>
       </c>
       <c r="L52" t="s">
-        <v>234</v>
+        <v>20</v>
       </c>
       <c r="M52" t="s">
         <v>21</v>
       </c>
       <c r="N52" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="O52" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53">
@@ -3668,31 +3530,31 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="n">
-        <v>145.0</v>
+        <v>148.0</v>
       </c>
       <c r="C53" t="n">
         <v>1.0</v>
       </c>
       <c r="D53" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E53" t="n">
-        <v>4.16564537E8</v>
+        <v>4.12306752E8</v>
       </c>
       <c r="F53" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="G53" t="s">
-        <v>29</v>
+        <v>251</v>
       </c>
       <c r="H53" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="I53" t="n">
-        <v>5.0354754E7</v>
+        <v>4.9532922E7</v>
       </c>
       <c r="J53" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="K53" t="s">
         <v>19</v>
@@ -3704,10 +3566,10 @@
         <v>21</v>
       </c>
       <c r="N53" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="O53" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54">
@@ -3715,7 +3577,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="n">
-        <v>145.0</v>
+        <v>150.0</v>
       </c>
       <c r="C54" t="n">
         <v>1.0</v>
@@ -3724,22 +3586,22 @@
         <v>1.0</v>
       </c>
       <c r="E54" t="n">
-        <v>4.16989412E8</v>
+        <v>3.7574279E8</v>
       </c>
       <c r="F54" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="G54" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="H54" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="I54" t="n">
-        <v>5.0447515E7</v>
+        <v>4.6510933E7</v>
       </c>
       <c r="J54" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="K54" t="s">
         <v>19</v>
@@ -3751,10 +3613,10 @@
         <v>21</v>
       </c>
       <c r="N54" t="s">
-        <v>153</v>
+        <v>260</v>
       </c>
       <c r="O54" t="s">
-        <v>153</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55">
@@ -3762,31 +3624,31 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="n">
-        <v>146.0</v>
+        <v>150.0</v>
       </c>
       <c r="C55" t="n">
         <v>1.0</v>
       </c>
       <c r="D55" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E55" t="n">
-        <v>3.41956905E8</v>
+        <v>4.05608703E8</v>
       </c>
       <c r="F55" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="G55" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="H55" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="I55" t="n">
-        <v>4.5543022E7</v>
+        <v>4.7665476E7</v>
       </c>
       <c r="J55" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="K55" t="s">
         <v>19</v>
@@ -3798,10 +3660,10 @@
         <v>21</v>
       </c>
       <c r="N55" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="O55" t="s">
-        <v>257</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56">
@@ -3809,31 +3671,31 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="n">
-        <v>146.0</v>
+        <v>152.0</v>
       </c>
       <c r="C56" t="n">
         <v>1.0</v>
       </c>
       <c r="D56" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="E56" t="n">
-        <v>3.63886455E8</v>
+        <v>3.41758296E8</v>
       </c>
       <c r="F56" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="G56" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="H56" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="I56" t="n">
-        <v>4.597992E7</v>
+        <v>4.5448221E7</v>
       </c>
       <c r="J56" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="K56" t="s">
         <v>19</v>
@@ -3845,10 +3707,10 @@
         <v>21</v>
       </c>
       <c r="N56" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="O56" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row r="57">
@@ -3856,31 +3718,31 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="n">
-        <v>146.0</v>
+        <v>152.0</v>
       </c>
       <c r="C57" t="n">
         <v>1.0</v>
       </c>
       <c r="D57" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="E57" t="n">
-        <v>4.11517077E8</v>
+        <v>3.65836212E8</v>
       </c>
       <c r="F57" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="G57" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
       <c r="H57" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="I57" t="n">
-        <v>4.936146E7</v>
+        <v>4.6338453E7</v>
       </c>
       <c r="J57" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="K57" t="s">
         <v>19</v>
@@ -3892,10 +3754,10 @@
         <v>21</v>
       </c>
       <c r="N57" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="O57" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="58">
@@ -3903,31 +3765,31 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="n">
-        <v>147.0</v>
+        <v>152.0</v>
       </c>
       <c r="C58" t="n">
         <v>1.0</v>
       </c>
       <c r="D58" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E58" t="n">
-        <v>4.25429398E8</v>
+        <v>4.14727847E8</v>
       </c>
       <c r="F58" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="G58" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="H58" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="I58" t="n">
-        <v>5.2254308E7</v>
+        <v>5.0011E7</v>
       </c>
       <c r="J58" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="K58" t="s">
         <v>19</v>
@@ -3939,10 +3801,10 @@
         <v>21</v>
       </c>
       <c r="N58" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O58" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59">
@@ -3950,31 +3812,31 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="n">
-        <v>148.0</v>
+        <v>153.0</v>
       </c>
       <c r="C59" t="n">
         <v>1.0</v>
       </c>
       <c r="D59" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="E59" t="n">
-        <v>3.36658357E8</v>
+        <v>3.36768E8</v>
       </c>
       <c r="F59" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="G59" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="H59" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="I59" t="n">
-        <v>4.4215146E7</v>
+        <v>4.4316677E7</v>
       </c>
       <c r="J59" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="K59" t="s">
         <v>19</v>
@@ -3986,10 +3848,10 @@
         <v>21</v>
       </c>
       <c r="N59" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="O59" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60">
@@ -3997,31 +3859,31 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="n">
-        <v>148.0</v>
+        <v>157.0</v>
       </c>
       <c r="C60" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="D60" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="E60" t="n">
-        <v>4.12306752E8</v>
+        <v>3.23894827E8</v>
       </c>
       <c r="F60" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="G60" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="H60" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="I60" t="n">
-        <v>4.9532922E7</v>
+        <v>4.253307E7</v>
       </c>
       <c r="J60" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="K60" t="s">
         <v>19</v>
@@ -4033,10 +3895,10 @@
         <v>21</v>
       </c>
       <c r="N60" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="O60" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61">
@@ -4044,31 +3906,31 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="n">
-        <v>150.0</v>
+        <v>158.0</v>
       </c>
       <c r="C61" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="D61" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E61" t="n">
-        <v>3.7574279E8</v>
+        <v>3.36933784E8</v>
       </c>
       <c r="F61" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="G61" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="H61" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I61" t="n">
-        <v>4.6510933E7</v>
+        <v>4.4268992E7</v>
       </c>
       <c r="J61" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="K61" t="s">
         <v>19</v>
@@ -4080,10 +3942,10 @@
         <v>21</v>
       </c>
       <c r="N61" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="O61" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="62">
@@ -4091,31 +3953,31 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="n">
-        <v>150.0</v>
+        <v>162.0</v>
       </c>
       <c r="C62" t="n">
-        <v>1.0</v>
+        <v>20.0</v>
       </c>
       <c r="D62" t="n">
         <v>3.0</v>
       </c>
       <c r="E62" t="n">
-        <v>4.05608703E8</v>
+        <v>4.11519961E8</v>
       </c>
       <c r="F62" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="G62" t="s">
-        <v>290</v>
+        <v>16</v>
       </c>
       <c r="H62" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="I62" t="n">
-        <v>4.7665476E7</v>
+        <v>4.9362666E7</v>
       </c>
       <c r="J62" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="K62" t="s">
         <v>19</v>
@@ -4127,10 +3989,10 @@
         <v>21</v>
       </c>
       <c r="N62" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="O62" t="s">
-        <v>176</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63">
@@ -4138,46 +4000,46 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="n">
-        <v>152.0</v>
+        <v>162.0</v>
       </c>
       <c r="C63" t="n">
-        <v>1.0</v>
+        <v>20.0</v>
       </c>
       <c r="D63" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="E63" t="n">
-        <v>3.41758296E8</v>
+        <v>4.39644406E8</v>
       </c>
       <c r="F63" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="G63" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="H63" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="I63" t="n">
-        <v>4.5448221E7</v>
+        <v>5.29921E7</v>
       </c>
       <c r="J63" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="K63" t="s">
-        <v>19</v>
+        <v>305</v>
       </c>
       <c r="L63" t="s">
         <v>20</v>
       </c>
       <c r="M63" t="s">
-        <v>21</v>
+        <v>306</v>
       </c>
       <c r="N63" t="s">
-        <v>298</v>
+        <v>16</v>
       </c>
       <c r="O63" t="s">
-        <v>298</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64">
@@ -4185,46 +4047,46 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="n">
-        <v>152.0</v>
+        <v>163.0</v>
       </c>
       <c r="C64" t="n">
-        <v>1.0</v>
+        <v>20.0</v>
       </c>
       <c r="D64" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E64" t="n">
-        <v>3.65836212E8</v>
+        <v>4.25515059E8</v>
       </c>
       <c r="F64" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="G64" t="s">
-        <v>159</v>
+        <v>308</v>
       </c>
       <c r="H64" t="s">
+        <v>309</v>
+      </c>
+      <c r="I64" t="n">
+        <v>5.2279275E7</v>
+      </c>
+      <c r="J64" t="s">
+        <v>310</v>
+      </c>
+      <c r="K64" t="s">
+        <v>305</v>
+      </c>
+      <c r="L64" t="s">
+        <v>20</v>
+      </c>
+      <c r="M64" t="s">
+        <v>306</v>
+      </c>
+      <c r="N64" t="s">
         <v>300</v>
       </c>
-      <c r="I64" t="n">
-        <v>4.6338453E7</v>
-      </c>
-      <c r="J64" t="s">
-        <v>301</v>
-      </c>
-      <c r="K64" t="s">
-        <v>19</v>
-      </c>
-      <c r="L64" t="s">
-        <v>20</v>
-      </c>
-      <c r="M64" t="s">
-        <v>21</v>
-      </c>
-      <c r="N64" t="s">
-        <v>302</v>
-      </c>
       <c r="O64" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65">
@@ -4232,46 +4094,46 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="n">
-        <v>152.0</v>
+        <v>163.0</v>
       </c>
       <c r="C65" t="n">
-        <v>1.0</v>
+        <v>20.0</v>
       </c>
       <c r="D65" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="E65" t="n">
-        <v>4.14727847E8</v>
+        <v>4.39644406E8</v>
       </c>
       <c r="F65" t="s">
+        <v>301</v>
+      </c>
+      <c r="G65" t="s">
+        <v>302</v>
+      </c>
+      <c r="H65" t="s">
         <v>303</v>
       </c>
-      <c r="G65" t="s">
+      <c r="I65" t="n">
+        <v>5.29921E7</v>
+      </c>
+      <c r="J65" t="s">
         <v>304</v>
       </c>
-      <c r="H65" t="s">
+      <c r="K65" t="s">
         <v>305</v>
       </c>
-      <c r="I65" t="n">
-        <v>5.0011E7</v>
-      </c>
-      <c r="J65" t="s">
+      <c r="L65" t="s">
+        <v>20</v>
+      </c>
+      <c r="M65" t="s">
         <v>306</v>
       </c>
-      <c r="K65" t="s">
-        <v>19</v>
-      </c>
-      <c r="L65" t="s">
-        <v>20</v>
-      </c>
-      <c r="M65" t="s">
-        <v>21</v>
-      </c>
       <c r="N65" t="s">
-        <v>307</v>
+        <v>16</v>
       </c>
       <c r="O65" t="s">
-        <v>307</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66">
@@ -4279,46 +4141,46 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="n">
-        <v>153.0</v>
+        <v>166.0</v>
       </c>
       <c r="C66" t="n">
-        <v>1.0</v>
+        <v>20.0</v>
       </c>
       <c r="D66" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E66" t="n">
-        <v>3.36768E8</v>
+        <v>4.47233337E8</v>
       </c>
       <c r="F66" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="G66" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="H66" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I66" t="n">
-        <v>4.4316677E7</v>
+        <v>5.130661E7</v>
       </c>
       <c r="J66" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="K66" t="s">
-        <v>19</v>
+        <v>305</v>
       </c>
       <c r="L66" t="s">
         <v>20</v>
       </c>
       <c r="M66" t="s">
-        <v>21</v>
+        <v>306</v>
       </c>
       <c r="N66" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O66" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="67">
@@ -4326,46 +4188,46 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="n">
-        <v>155.0</v>
+        <v>184.0</v>
       </c>
       <c r="C67" t="n">
-        <v>9.0</v>
+        <v>20.0</v>
       </c>
       <c r="D67" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="E67" t="n">
-        <v>3.36846155E8</v>
+        <v>4.18463807E8</v>
       </c>
       <c r="F67" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="G67" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="H67" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="I67" t="n">
-        <v>4.4296948E7</v>
+        <v>5.077581E7</v>
       </c>
       <c r="J67" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="K67" t="s">
-        <v>19</v>
+        <v>305</v>
       </c>
       <c r="L67" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="M67" t="s">
-        <v>21</v>
+        <v>306</v>
       </c>
       <c r="N67" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="O67" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="68">
@@ -4373,43 +4235,43 @@
         <v>67.0</v>
       </c>
       <c r="B68" t="n">
-        <v>155.0</v>
+        <v>184.0</v>
       </c>
       <c r="C68" t="n">
-        <v>9.0</v>
+        <v>20.0</v>
       </c>
       <c r="D68" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="E68" t="n">
-        <v>3.38984593E8</v>
+        <v>4.42647888E8</v>
       </c>
       <c r="F68" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="G68" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="H68" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="I68" t="n">
-        <v>4.4603578E7</v>
+        <v>5.077581E7</v>
       </c>
       <c r="J68" t="s">
+        <v>327</v>
+      </c>
+      <c r="K68" t="s">
+        <v>328</v>
+      </c>
+      <c r="L68" t="s">
+        <v>20</v>
+      </c>
+      <c r="M68" t="s">
+        <v>21</v>
+      </c>
+      <c r="N68" t="s">
         <v>322</v>
-      </c>
-      <c r="K68" t="s">
-        <v>19</v>
-      </c>
-      <c r="L68" t="s">
-        <v>20</v>
-      </c>
-      <c r="M68" t="s">
-        <v>21</v>
-      </c>
-      <c r="N68" t="s">
-        <v>323</v>
       </c>
       <c r="O68" t="s">
         <v>323</v>
@@ -4420,46 +4282,46 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="n">
-        <v>155.0</v>
+        <v>184.0</v>
       </c>
       <c r="C69" t="n">
-        <v>9.0</v>
+        <v>20.0</v>
       </c>
       <c r="D69" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="E69" t="n">
-        <v>3.52999186E8</v>
+        <v>4.50570801E8</v>
       </c>
       <c r="F69" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="G69" t="s">
-        <v>226</v>
+        <v>330</v>
       </c>
       <c r="H69" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I69" t="n">
-        <v>4.58261E7</v>
+        <v>5.077581E7</v>
       </c>
       <c r="J69" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="K69" t="s">
-        <v>19</v>
+        <v>333</v>
       </c>
       <c r="L69" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="M69" t="s">
         <v>21</v>
       </c>
       <c r="N69" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="O69" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70">
@@ -4467,563 +4329,46 @@
         <v>69.0</v>
       </c>
       <c r="B70" t="n">
-        <v>155.0</v>
+        <v>199.0</v>
       </c>
       <c r="C70" t="n">
-        <v>9.0</v>
+        <v>20.0</v>
       </c>
       <c r="D70" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="E70" t="n">
-        <v>4.05512845E8</v>
+        <v>4.50570801E8</v>
       </c>
       <c r="F70" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G70" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H70" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I70" t="n">
-        <v>4.7972641E7</v>
+        <v>5.077581E7</v>
       </c>
       <c r="J70" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K70" t="s">
-        <v>19</v>
+        <v>333</v>
       </c>
       <c r="L70" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="M70" t="s">
         <v>21</v>
       </c>
       <c r="N70" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="O70" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="B71" t="n">
-        <v>157.0</v>
-      </c>
-      <c r="C71" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="D71" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="E71" t="n">
-        <v>3.23894827E8</v>
-      </c>
-      <c r="F71" t="s">
-        <v>333</v>
-      </c>
-      <c r="G71" t="s">
-        <v>334</v>
-      </c>
-      <c r="H71" t="s">
-        <v>335</v>
-      </c>
-      <c r="I71" t="n">
-        <v>4.253307E7</v>
-      </c>
-      <c r="J71" t="s">
-        <v>336</v>
-      </c>
-      <c r="K71" t="s">
-        <v>19</v>
-      </c>
-      <c r="L71" t="s">
-        <v>20</v>
-      </c>
-      <c r="M71" t="s">
-        <v>21</v>
-      </c>
-      <c r="N71" t="s">
-        <v>337</v>
-      </c>
-      <c r="O71" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>71.0</v>
-      </c>
-      <c r="B72" t="n">
-        <v>158.0</v>
-      </c>
-      <c r="C72" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="D72" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E72" t="n">
-        <v>3.36933784E8</v>
-      </c>
-      <c r="F72" t="s">
-        <v>338</v>
-      </c>
-      <c r="G72" t="s">
-        <v>339</v>
-      </c>
-      <c r="H72" t="s">
-        <v>340</v>
-      </c>
-      <c r="I72" t="n">
-        <v>4.4268992E7</v>
-      </c>
-      <c r="J72" t="s">
-        <v>341</v>
-      </c>
-      <c r="K72" t="s">
-        <v>19</v>
-      </c>
-      <c r="L72" t="s">
-        <v>20</v>
-      </c>
-      <c r="M72" t="s">
-        <v>21</v>
-      </c>
-      <c r="N72" t="s">
-        <v>342</v>
-      </c>
-      <c r="O72" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="B73" t="n">
-        <v>162.0</v>
-      </c>
-      <c r="C73" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D73" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E73" t="n">
-        <v>4.11519961E8</v>
-      </c>
-      <c r="F73" t="s">
-        <v>343</v>
-      </c>
-      <c r="G73" t="s">
-        <v>16</v>
-      </c>
-      <c r="H73" t="s">
-        <v>344</v>
-      </c>
-      <c r="I73" t="n">
-        <v>4.9362666E7</v>
-      </c>
-      <c r="J73" t="s">
-        <v>345</v>
-      </c>
-      <c r="K73" t="s">
-        <v>19</v>
-      </c>
-      <c r="L73" t="s">
-        <v>20</v>
-      </c>
-      <c r="M73" t="s">
-        <v>21</v>
-      </c>
-      <c r="N73" t="s">
-        <v>346</v>
-      </c>
-      <c r="O73" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>73.0</v>
-      </c>
-      <c r="B74" t="n">
-        <v>162.0</v>
-      </c>
-      <c r="C74" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D74" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E74" t="n">
-        <v>4.39644406E8</v>
-      </c>
-      <c r="F74" t="s">
-        <v>347</v>
-      </c>
-      <c r="G74" t="s">
-        <v>348</v>
-      </c>
-      <c r="H74" t="s">
-        <v>349</v>
-      </c>
-      <c r="I74" t="n">
-        <v>5.29921E7</v>
-      </c>
-      <c r="J74" t="s">
-        <v>350</v>
-      </c>
-      <c r="K74" t="s">
-        <v>351</v>
-      </c>
-      <c r="L74" t="s">
-        <v>20</v>
-      </c>
-      <c r="M74" t="s">
-        <v>352</v>
-      </c>
-      <c r="N74" t="s">
-        <v>16</v>
-      </c>
-      <c r="O74" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>74.0</v>
-      </c>
-      <c r="B75" t="n">
-        <v>163.0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D75" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E75" t="n">
-        <v>4.25515059E8</v>
-      </c>
-      <c r="F75" t="s">
-        <v>353</v>
-      </c>
-      <c r="G75" t="s">
-        <v>354</v>
-      </c>
-      <c r="H75" t="s">
-        <v>355</v>
-      </c>
-      <c r="I75" t="n">
-        <v>5.2279275E7</v>
-      </c>
-      <c r="J75" t="s">
-        <v>356</v>
-      </c>
-      <c r="K75" t="s">
-        <v>351</v>
-      </c>
-      <c r="L75" t="s">
-        <v>20</v>
-      </c>
-      <c r="M75" t="s">
-        <v>352</v>
-      </c>
-      <c r="N75" t="s">
-        <v>346</v>
-      </c>
-      <c r="O75" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>75.0</v>
-      </c>
-      <c r="B76" t="n">
-        <v>163.0</v>
-      </c>
-      <c r="C76" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D76" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E76" t="n">
-        <v>4.39644406E8</v>
-      </c>
-      <c r="F76" t="s">
-        <v>347</v>
-      </c>
-      <c r="G76" t="s">
-        <v>348</v>
-      </c>
-      <c r="H76" t="s">
-        <v>349</v>
-      </c>
-      <c r="I76" t="n">
-        <v>5.29921E7</v>
-      </c>
-      <c r="J76" t="s">
-        <v>350</v>
-      </c>
-      <c r="K76" t="s">
-        <v>351</v>
-      </c>
-      <c r="L76" t="s">
-        <v>20</v>
-      </c>
-      <c r="M76" t="s">
-        <v>352</v>
-      </c>
-      <c r="N76" t="s">
-        <v>16</v>
-      </c>
-      <c r="O76" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>76.0</v>
-      </c>
-      <c r="B77" t="n">
-        <v>166.0</v>
-      </c>
-      <c r="C77" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D77" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E77" t="n">
-        <v>4.47233337E8</v>
-      </c>
-      <c r="F77" t="s">
-        <v>357</v>
-      </c>
-      <c r="G77" t="s">
-        <v>358</v>
-      </c>
-      <c r="H77" t="s">
-        <v>359</v>
-      </c>
-      <c r="I77" t="n">
-        <v>5.130661E7</v>
-      </c>
-      <c r="J77" t="s">
-        <v>360</v>
-      </c>
-      <c r="K77" t="s">
-        <v>351</v>
-      </c>
-      <c r="L77" t="s">
-        <v>20</v>
-      </c>
-      <c r="M77" t="s">
-        <v>352</v>
-      </c>
-      <c r="N77" t="s">
-        <v>361</v>
-      </c>
-      <c r="O77" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="B78" t="n">
-        <v>179.0</v>
-      </c>
-      <c r="C78" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D78" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="E78" t="n">
-        <v>4.18463807E8</v>
-      </c>
-      <c r="F78" t="s">
-        <v>363</v>
-      </c>
-      <c r="G78" t="s">
-        <v>364</v>
-      </c>
-      <c r="H78" t="s">
-        <v>365</v>
-      </c>
-      <c r="I78" t="n">
-        <v>5.077581E7</v>
-      </c>
-      <c r="J78" t="s">
-        <v>366</v>
-      </c>
-      <c r="K78" t="s">
-        <v>351</v>
-      </c>
-      <c r="L78" t="s">
-        <v>367</v>
-      </c>
-      <c r="M78" t="s">
-        <v>352</v>
-      </c>
-      <c r="N78" t="s">
-        <v>368</v>
-      </c>
-      <c r="O78" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="B79" t="n">
-        <v>179.0</v>
-      </c>
-      <c r="C79" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D79" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E79" t="n">
-        <v>4.42647888E8</v>
-      </c>
-      <c r="F79" t="s">
-        <v>370</v>
-      </c>
-      <c r="G79" t="s">
-        <v>371</v>
-      </c>
-      <c r="H79" t="s">
-        <v>372</v>
-      </c>
-      <c r="I79" t="n">
-        <v>5.077581E7</v>
-      </c>
-      <c r="J79" t="s">
-        <v>373</v>
-      </c>
-      <c r="K79" t="s">
-        <v>374</v>
-      </c>
-      <c r="L79" t="s">
-        <v>20</v>
-      </c>
-      <c r="M79" t="s">
-        <v>21</v>
-      </c>
-      <c r="N79" t="s">
-        <v>368</v>
-      </c>
-      <c r="O79" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>79.0</v>
-      </c>
-      <c r="B80" t="n">
-        <v>179.0</v>
-      </c>
-      <c r="C80" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="E80" t="n">
-        <v>4.50570801E8</v>
-      </c>
-      <c r="F80" t="s">
-        <v>375</v>
-      </c>
-      <c r="G80" t="s">
-        <v>376</v>
-      </c>
-      <c r="H80" t="s">
-        <v>377</v>
-      </c>
-      <c r="I80" t="n">
-        <v>5.077581E7</v>
-      </c>
-      <c r="J80" t="s">
-        <v>378</v>
-      </c>
-      <c r="K80" t="s">
-        <v>379</v>
-      </c>
-      <c r="L80" t="s">
-        <v>367</v>
-      </c>
-      <c r="M80" t="s">
-        <v>21</v>
-      </c>
-      <c r="N80" t="s">
-        <v>368</v>
-      </c>
-      <c r="O80" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="B81" t="n">
-        <v>194.0</v>
-      </c>
-      <c r="C81" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="D81" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="E81" t="n">
-        <v>4.50570801E8</v>
-      </c>
-      <c r="F81" t="s">
-        <v>375</v>
-      </c>
-      <c r="G81" t="s">
-        <v>376</v>
-      </c>
-      <c r="H81" t="s">
-        <v>377</v>
-      </c>
-      <c r="I81" t="n">
-        <v>5.077581E7</v>
-      </c>
-      <c r="J81" t="s">
-        <v>378</v>
-      </c>
-      <c r="K81" t="s">
-        <v>379</v>
-      </c>
-      <c r="L81" t="s">
-        <v>367</v>
-      </c>
-      <c r="M81" t="s">
-        <v>21</v>
-      </c>
-      <c r="N81" t="s">
-        <v>368</v>
-      </c>
-      <c r="O81" t="s">
-        <v>369</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>